<commit_message>
arreglo de bugs al cancelar las descargas
</commit_message>
<xml_diff>
--- a/escenario_2/export_dataframe.xlsx
+++ b/escenario_2/export_dataframe.xlsx
@@ -478,467 +478,467 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-97073</v>
+        <v>-111166</v>
       </c>
       <c r="B2" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C2" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="D2" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E2" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F2" t="n">
-        <v>81156</v>
+        <v>40497</v>
       </c>
       <c r="G2" t="n">
-        <v>2129.335745509432</v>
+        <v>4767.321649234811</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-111617</v>
+        <v>-119715</v>
       </c>
       <c r="B3" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C3" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D3" t="n">
         <v>60000</v>
       </c>
       <c r="E3" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F3" t="n">
-        <v>80646</v>
+        <v>39628</v>
       </c>
       <c r="G3" t="n">
-        <v>3600.193450257386</v>
+        <v>-41957.71296485801</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-121038</v>
+        <v>-100916</v>
       </c>
       <c r="B4" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C4" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D4" t="n">
         <v>30000</v>
       </c>
       <c r="E4" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F4" t="n">
-        <v>42272</v>
+        <v>44316</v>
       </c>
       <c r="G4" t="n">
-        <v>-36616.64154630309</v>
+        <v>-33394.62549296932</v>
       </c>
       <c r="H4" t="n">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-106708</v>
+        <v>-110652</v>
       </c>
       <c r="B5" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="C5" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D5" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E5" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F5" t="n">
-        <v>79857</v>
+        <v>60537</v>
       </c>
       <c r="G5" t="n">
-        <v>-10057.7987813044</v>
+        <v>-26296.25502964172</v>
       </c>
       <c r="H5" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-110475</v>
+        <v>-97947</v>
       </c>
       <c r="B6" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C6" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D6" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E6" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F6" t="n">
-        <v>81541</v>
+        <v>37616</v>
       </c>
       <c r="G6" t="n">
-        <v>-9825.926120952437</v>
+        <v>-14502.74288570416</v>
       </c>
       <c r="H6" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-87196</v>
+        <v>-104810</v>
       </c>
       <c r="B7" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="C7" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E7" t="n">
         <v>50000</v>
       </c>
       <c r="F7" t="n">
-        <v>41728</v>
+        <v>80180</v>
       </c>
       <c r="G7" t="n">
-        <v>-19940.07870465494</v>
+        <v>-8007.030463158371</v>
       </c>
       <c r="H7" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-106331</v>
+        <v>-110734</v>
       </c>
       <c r="B8" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C8" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D8" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E8" t="n">
         <v>20000</v>
       </c>
       <c r="F8" t="n">
-        <v>58115</v>
+        <v>53548</v>
       </c>
       <c r="G8" t="n">
-        <v>-32460.69520081234</v>
+        <v>-35949.26114637084</v>
       </c>
       <c r="H8" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-100950</v>
+        <v>-117473</v>
       </c>
       <c r="B9" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C9" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D9" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E9" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F9" t="n">
-        <v>50541</v>
+        <v>59315</v>
       </c>
       <c r="G9" t="n">
-        <v>-22979.22732073467</v>
+        <v>-2820.302087770953</v>
       </c>
       <c r="H9" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-106836</v>
+        <v>-94208</v>
       </c>
       <c r="B10" t="n">
         <v>30000</v>
       </c>
       <c r="C10" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D10" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="E10" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F10" t="n">
-        <v>61903</v>
+        <v>64284</v>
       </c>
       <c r="G10" t="n">
-        <v>-35739.47594492204</v>
+        <v>2348.126633903568</v>
       </c>
       <c r="H10" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-109897</v>
+        <v>-95225</v>
       </c>
       <c r="B11" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C11" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D11" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E11" t="n">
         <v>30000</v>
       </c>
       <c r="F11" t="n">
-        <v>38093</v>
+        <v>39125</v>
       </c>
       <c r="G11" t="n">
-        <v>-25278.23767215805</v>
+        <v>-6264.927099726179</v>
       </c>
       <c r="H11" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-112457</v>
+        <v>-127066</v>
       </c>
       <c r="B12" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C12" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D12" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E12" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F12" t="n">
-        <v>83278</v>
+        <v>48011</v>
       </c>
       <c r="G12" t="n">
-        <v>3497.489644217798</v>
+        <v>-53731.60419435684</v>
       </c>
       <c r="H12" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-90673</v>
+        <v>-114899</v>
       </c>
       <c r="B13" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C13" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D13" t="n">
         <v>60000</v>
       </c>
       <c r="E13" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F13" t="n">
-        <v>55174</v>
+        <v>48267</v>
       </c>
       <c r="G13" t="n">
-        <v>30209.56859072913</v>
+        <v>-39394.41668189845</v>
       </c>
       <c r="H13" t="n">
-        <v>0.16</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-105843</v>
+        <v>-90830</v>
       </c>
       <c r="B14" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C14" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D14" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E14" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F14" t="n">
-        <v>41040</v>
+        <v>50237</v>
       </c>
       <c r="G14" t="n">
-        <v>-5201.786445910277</v>
+        <v>-32367.0603710906</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-96161</v>
+        <v>-100931</v>
       </c>
       <c r="B15" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C15" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D15" t="n">
         <v>30000</v>
       </c>
       <c r="E15" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F15" t="n">
-        <v>69292</v>
+        <v>84852</v>
       </c>
       <c r="G15" t="n">
-        <v>-18395.2685599812</v>
+        <v>10957.7342711441</v>
       </c>
       <c r="H15" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-112399</v>
+        <v>-93237</v>
       </c>
       <c r="B16" t="n">
         <v>60000</v>
       </c>
       <c r="C16" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D16" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E16" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F16" t="n">
-        <v>80165</v>
+        <v>70357</v>
       </c>
       <c r="G16" t="n">
-        <v>15351.03508864969</v>
+        <v>28714.9646919414</v>
       </c>
       <c r="H16" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-96266</v>
+        <v>-111652</v>
       </c>
       <c r="B17" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C17" t="n">
         <v>30000</v>
       </c>
       <c r="D17" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E17" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F17" t="n">
-        <v>80640</v>
+        <v>59704</v>
       </c>
       <c r="G17" t="n">
-        <v>9510.293924231308</v>
+        <v>-53595.10999069365</v>
       </c>
       <c r="H17" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-102558</v>
+        <v>-90344</v>
       </c>
       <c r="B18" t="n">
         <v>30000</v>
       </c>
       <c r="C18" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D18" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E18" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F18" t="n">
-        <v>80721</v>
+        <v>44059</v>
       </c>
       <c r="G18" t="n">
-        <v>-27818.76676072255</v>
+        <v>-25453.58921025759</v>
       </c>
       <c r="H18" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-91387</v>
+        <v>-118559</v>
       </c>
       <c r="B19" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C19" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D19" t="n">
         <v>50000</v>
       </c>
       <c r="E19" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F19" t="n">
-        <v>47078</v>
+        <v>40999</v>
       </c>
       <c r="G19" t="n">
-        <v>141.7656543460471</v>
+        <v>-24407.49498253706</v>
       </c>
       <c r="H19" t="n">
         <v>0.21</v>
@@ -946,39 +946,39 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-91018</v>
+        <v>-102141</v>
       </c>
       <c r="B20" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C20" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D20" t="n">
         <v>60000</v>
       </c>
       <c r="E20" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="F20" t="n">
-        <v>40650</v>
+        <v>64775</v>
       </c>
       <c r="G20" t="n">
-        <v>19299.14688917161</v>
+        <v>-16707.31080287175</v>
       </c>
       <c r="H20" t="n">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>-108839</v>
+        <v>-100072</v>
       </c>
       <c r="B21" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C21" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D21" t="n">
         <v>30000</v>
@@ -987,114 +987,114 @@
         <v>20000</v>
       </c>
       <c r="F21" t="n">
-        <v>69454</v>
+        <v>73517</v>
       </c>
       <c r="G21" t="n">
-        <v>-28134.60411784296</v>
+        <v>-3818.087548277781</v>
       </c>
       <c r="H21" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>-115947</v>
+        <v>-108312</v>
       </c>
       <c r="B22" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C22" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D22" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E22" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F22" t="n">
-        <v>38168</v>
+        <v>69940</v>
       </c>
       <c r="G22" t="n">
-        <v>-18900.51937987273</v>
+        <v>-29647.10330246377</v>
       </c>
       <c r="H22" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>-97507</v>
+        <v>-124211</v>
       </c>
       <c r="B23" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C23" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D23" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E23" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F23" t="n">
-        <v>39922</v>
+        <v>42981</v>
       </c>
       <c r="G23" t="n">
-        <v>3624.551660581828</v>
+        <v>-32031.42945585073</v>
       </c>
       <c r="H23" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>-104154</v>
+        <v>-108723</v>
       </c>
       <c r="B24" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C24" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D24" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E24" t="n">
         <v>30000</v>
       </c>
       <c r="F24" t="n">
-        <v>74249</v>
+        <v>79452</v>
       </c>
       <c r="G24" t="n">
-        <v>-13958.1560925979</v>
+        <v>-21116.52703061449</v>
       </c>
       <c r="H24" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>-102986</v>
+        <v>-105082</v>
       </c>
       <c r="B25" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C25" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D25" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E25" t="n">
         <v>50000</v>
       </c>
       <c r="F25" t="n">
-        <v>53443</v>
+        <v>68442</v>
       </c>
       <c r="G25" t="n">
-        <v>-3050.355849897558</v>
+        <v>2497.546528830993</v>
       </c>
       <c r="H25" t="n">
         <v>0.23</v>
@@ -1102,207 +1102,207 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>-114638</v>
+        <v>-87094</v>
       </c>
       <c r="B26" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C26" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D26" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E26" t="n">
         <v>60000</v>
       </c>
       <c r="F26" t="n">
-        <v>41438</v>
+        <v>81746</v>
       </c>
       <c r="G26" t="n">
-        <v>-25872.29537429404</v>
+        <v>25940.0510228132</v>
       </c>
       <c r="H26" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-115088</v>
+        <v>-118292</v>
       </c>
       <c r="B27" t="n">
         <v>30000</v>
       </c>
       <c r="C27" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D27" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E27" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F27" t="n">
-        <v>60483</v>
+        <v>41010</v>
       </c>
       <c r="G27" t="n">
-        <v>-35322.01955480878</v>
+        <v>-52792.26507518956</v>
       </c>
       <c r="H27" t="n">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-98769</v>
+        <v>-108352</v>
       </c>
       <c r="B28" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C28" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D28" t="n">
         <v>30000</v>
       </c>
       <c r="E28" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F28" t="n">
-        <v>83980</v>
+        <v>59230</v>
       </c>
       <c r="G28" t="n">
-        <v>-4127.702584503395</v>
+        <v>-23598.88413503208</v>
       </c>
       <c r="H28" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-89910</v>
+        <v>-102809</v>
       </c>
       <c r="B29" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C29" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D29" t="n">
         <v>50000</v>
       </c>
       <c r="E29" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F29" t="n">
-        <v>58894</v>
+        <v>58693</v>
       </c>
       <c r="G29" t="n">
-        <v>6390.389117072631</v>
+        <v>14865.17717182684</v>
       </c>
       <c r="H29" t="n">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>-104029</v>
+        <v>-104372</v>
       </c>
       <c r="B30" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C30" t="n">
         <v>30000</v>
       </c>
       <c r="D30" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E30" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F30" t="n">
-        <v>74669</v>
+        <v>66667</v>
       </c>
       <c r="G30" t="n">
-        <v>-4898.631665716028</v>
+        <v>-10419.09515386966</v>
       </c>
       <c r="H30" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-104834</v>
+        <v>-97929</v>
       </c>
       <c r="B31" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C31" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D31" t="n">
         <v>30000</v>
       </c>
       <c r="E31" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F31" t="n">
-        <v>45747</v>
+        <v>58123</v>
       </c>
       <c r="G31" t="n">
-        <v>-53769.00149401415</v>
+        <v>-13082.69107964482</v>
       </c>
       <c r="H31" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-105020</v>
+        <v>-109635</v>
       </c>
       <c r="B32" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C32" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D32" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E32" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F32" t="n">
-        <v>54103</v>
+        <v>48950</v>
       </c>
       <c r="G32" t="n">
-        <v>-20571.30995856105</v>
+        <v>-23643.20352761883</v>
       </c>
       <c r="H32" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-99644</v>
+        <v>-98911</v>
       </c>
       <c r="B33" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="C33" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D33" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E33" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F33" t="n">
-        <v>68415</v>
+        <v>60631</v>
       </c>
       <c r="G33" t="n">
-        <v>-36073.93756647723</v>
+        <v>21378.42075759919</v>
       </c>
       <c r="H33" t="n">
         <v>0.21</v>
@@ -1310,25 +1310,25 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-99827</v>
+        <v>-110593</v>
       </c>
       <c r="B34" t="n">
         <v>60000</v>
       </c>
       <c r="C34" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D34" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E34" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F34" t="n">
-        <v>37117</v>
+        <v>46839</v>
       </c>
       <c r="G34" t="n">
-        <v>-3419.992796059161</v>
+        <v>-5534.851727173271</v>
       </c>
       <c r="H34" t="n">
         <v>0.21</v>
@@ -1336,233 +1336,233 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-87592</v>
+        <v>-108244</v>
       </c>
       <c r="B35" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C35" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D35" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E35" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F35" t="n">
-        <v>42942</v>
+        <v>80456</v>
       </c>
       <c r="G35" t="n">
-        <v>17524.55619666036</v>
+        <v>-22493.44887999741</v>
       </c>
       <c r="H35" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>-125578</v>
+        <v>-93767</v>
       </c>
       <c r="B36" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C36" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D36" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E36" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F36" t="n">
-        <v>71897</v>
+        <v>38658</v>
       </c>
       <c r="G36" t="n">
-        <v>-31852.64462670432</v>
+        <v>-47776.78303859817</v>
       </c>
       <c r="H36" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-105660</v>
+        <v>-101088</v>
       </c>
       <c r="B37" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C37" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D37" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="E37" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F37" t="n">
-        <v>80545</v>
+        <v>49503</v>
       </c>
       <c r="G37" t="n">
-        <v>3479.218595463317</v>
+        <v>-37459.17084409539</v>
       </c>
       <c r="H37" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>-114230</v>
+        <v>-122805</v>
       </c>
       <c r="B38" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C38" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D38" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E38" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F38" t="n">
-        <v>60161</v>
+        <v>70852</v>
       </c>
       <c r="G38" t="n">
-        <v>-17708.59120510862</v>
+        <v>-44557.19283825087</v>
       </c>
       <c r="H38" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-119808</v>
+        <v>-96925</v>
       </c>
       <c r="B39" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C39" t="n">
         <v>20000</v>
       </c>
       <c r="D39" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E39" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F39" t="n">
-        <v>57585</v>
+        <v>64566</v>
       </c>
       <c r="G39" t="n">
-        <v>-51884.96599692643</v>
+        <v>-33243.70924331572</v>
       </c>
       <c r="H39" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>-110131</v>
+        <v>-86454</v>
       </c>
       <c r="B40" t="n">
         <v>30000</v>
       </c>
       <c r="C40" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D40" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E40" t="n">
         <v>40000</v>
       </c>
       <c r="F40" t="n">
-        <v>48545</v>
+        <v>58354</v>
       </c>
       <c r="G40" t="n">
-        <v>-31438.91107307912</v>
+        <v>-12238.17081696276</v>
       </c>
       <c r="H40" t="n">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>-107269</v>
+        <v>-114010</v>
       </c>
       <c r="B41" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C41" t="n">
         <v>30000</v>
       </c>
       <c r="D41" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E41" t="n">
         <v>30000</v>
       </c>
       <c r="F41" t="n">
-        <v>80497</v>
+        <v>50938</v>
       </c>
       <c r="G41" t="n">
-        <v>-28677.63049458242</v>
+        <v>-27913.4426988749</v>
       </c>
       <c r="H41" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>-110097</v>
+        <v>-103474</v>
       </c>
       <c r="B42" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C42" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D42" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E42" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F42" t="n">
-        <v>54441</v>
+        <v>49929</v>
       </c>
       <c r="G42" t="n">
-        <v>437.8306004396327</v>
+        <v>-28506.36288787763</v>
       </c>
       <c r="H42" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>-90712</v>
+        <v>-99352</v>
       </c>
       <c r="B43" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C43" t="n">
         <v>60000</v>
       </c>
       <c r="D43" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E43" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F43" t="n">
-        <v>60985</v>
+        <v>78009</v>
       </c>
       <c r="G43" t="n">
-        <v>1414.247978490166</v>
+        <v>-17320.34941885038</v>
       </c>
       <c r="H43" t="n">
         <v>0.23</v>
@@ -1570,337 +1570,337 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>-98917</v>
+        <v>-109229</v>
       </c>
       <c r="B44" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C44" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D44" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E44" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F44" t="n">
-        <v>43248</v>
+        <v>80907</v>
       </c>
       <c r="G44" t="n">
-        <v>16185.51113408233</v>
+        <v>-31031.37047153969</v>
       </c>
       <c r="H44" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>-106210</v>
+        <v>-101333</v>
       </c>
       <c r="B45" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C45" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="D45" t="n">
         <v>50000</v>
       </c>
       <c r="E45" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F45" t="n">
-        <v>79032</v>
+        <v>51257</v>
       </c>
       <c r="G45" t="n">
-        <v>-5073.595894991651</v>
+        <v>-30489.09608159261</v>
       </c>
       <c r="H45" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>-89032</v>
+        <v>-92394</v>
       </c>
       <c r="B46" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C46" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D46" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E46" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F46" t="n">
-        <v>77097</v>
+        <v>52042</v>
       </c>
       <c r="G46" t="n">
-        <v>5150.733277329529</v>
+        <v>-36405.39240979103</v>
       </c>
       <c r="H46" t="n">
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>-89268</v>
+        <v>-112660</v>
       </c>
       <c r="B47" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C47" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D47" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E47" t="n">
         <v>40000</v>
       </c>
       <c r="F47" t="n">
-        <v>78328</v>
+        <v>78449</v>
       </c>
       <c r="G47" t="n">
-        <v>4693.4836461671</v>
+        <v>-16941.51929581302</v>
       </c>
       <c r="H47" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>-101135</v>
+        <v>-102941</v>
       </c>
       <c r="B48" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C48" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D48" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E48" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F48" t="n">
-        <v>81503</v>
+        <v>80814</v>
       </c>
       <c r="G48" t="n">
-        <v>-6352.411342309333</v>
+        <v>-25118.57124298393</v>
       </c>
       <c r="H48" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>-101500</v>
+        <v>-103655</v>
       </c>
       <c r="B49" t="n">
         <v>40000</v>
       </c>
       <c r="C49" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D49" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E49" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F49" t="n">
-        <v>72572</v>
+        <v>53809</v>
       </c>
       <c r="G49" t="n">
-        <v>-5765.171112594116</v>
+        <v>-17207.18057440033</v>
       </c>
       <c r="H49" t="n">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>-97239</v>
+        <v>-95730</v>
       </c>
       <c r="B50" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C50" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D50" t="n">
         <v>40000</v>
       </c>
       <c r="E50" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F50" t="n">
-        <v>44633</v>
+        <v>50459</v>
       </c>
       <c r="G50" t="n">
-        <v>-6567.572863535339</v>
+        <v>-17997.53549233059</v>
       </c>
       <c r="H50" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>-87789</v>
+        <v>-95992</v>
       </c>
       <c r="B51" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C51" t="n">
         <v>40000</v>
       </c>
       <c r="D51" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E51" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F51" t="n">
-        <v>61302</v>
+        <v>40512</v>
       </c>
       <c r="G51" t="n">
-        <v>-8731.735664968168</v>
+        <v>6636.839722150153</v>
       </c>
       <c r="H51" t="n">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>-88102</v>
+        <v>-98248</v>
       </c>
       <c r="B52" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C52" t="n">
         <v>20000</v>
       </c>
       <c r="D52" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E52" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F52" t="n">
-        <v>58338</v>
+        <v>50956</v>
       </c>
       <c r="G52" t="n">
-        <v>-1384.530601457211</v>
+        <v>-32409.25165215396</v>
       </c>
       <c r="H52" t="n">
-        <v>0.18</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>-93955</v>
+        <v>-114556</v>
       </c>
       <c r="B53" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C53" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D53" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E53" t="n">
         <v>50000</v>
       </c>
       <c r="F53" t="n">
-        <v>36792</v>
+        <v>67747</v>
       </c>
       <c r="G53" t="n">
-        <v>1997.985594536208</v>
+        <v>858.4511292104435</v>
       </c>
       <c r="H53" t="n">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>-98979</v>
+        <v>-121301</v>
       </c>
       <c r="B54" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C54" t="n">
         <v>20000</v>
       </c>
       <c r="D54" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E54" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F54" t="n">
-        <v>83634</v>
+        <v>41007</v>
       </c>
       <c r="G54" t="n">
-        <v>3839.512942735164</v>
+        <v>-69602.20771117421</v>
       </c>
       <c r="H54" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>-90399</v>
+        <v>-98367</v>
       </c>
       <c r="B55" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C55" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D55" t="n">
         <v>60000</v>
       </c>
       <c r="E55" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F55" t="n">
-        <v>53354</v>
+        <v>60995</v>
       </c>
       <c r="G55" t="n">
-        <v>-15518.15524832662</v>
+        <v>-15233.41859220002</v>
       </c>
       <c r="H55" t="n">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>-88610</v>
+        <v>-105105</v>
       </c>
       <c r="B56" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C56" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="D56" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E56" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F56" t="n">
-        <v>38720</v>
+        <v>62242</v>
       </c>
       <c r="G56" t="n">
-        <v>-9340.557694558889</v>
+        <v>4399.205389714674</v>
       </c>
       <c r="H56" t="n">
         <v>0.22</v>
@@ -1908,13 +1908,13 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>-98678</v>
+        <v>-83190</v>
       </c>
       <c r="B57" t="n">
         <v>50000</v>
       </c>
       <c r="C57" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D57" t="n">
         <v>60000</v>
@@ -1923,180 +1923,180 @@
         <v>30000</v>
       </c>
       <c r="F57" t="n">
-        <v>83265</v>
+        <v>39954</v>
       </c>
       <c r="G57" t="n">
-        <v>16798.88293810537</v>
+        <v>9587.227544618394</v>
       </c>
       <c r="H57" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>-119637</v>
+        <v>-95742</v>
       </c>
       <c r="B58" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C58" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D58" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E58" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F58" t="n">
-        <v>71196</v>
+        <v>60508</v>
       </c>
       <c r="G58" t="n">
-        <v>-25103.20503907767</v>
+        <v>-35537.1929291237</v>
       </c>
       <c r="H58" t="n">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>-103325</v>
+        <v>-105531</v>
       </c>
       <c r="B59" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="C59" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D59" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E59" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F59" t="n">
-        <v>52267</v>
+        <v>52197</v>
       </c>
       <c r="G59" t="n">
-        <v>-35257.24251560518</v>
+        <v>-13311.34748499166</v>
       </c>
       <c r="H59" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>-112355</v>
+        <v>-120602</v>
       </c>
       <c r="B60" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C60" t="n">
         <v>60000</v>
       </c>
       <c r="D60" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E60" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F60" t="n">
-        <v>70800</v>
+        <v>69474</v>
       </c>
       <c r="G60" t="n">
-        <v>-8208.453034856568</v>
+        <v>-33374.29284342394</v>
       </c>
       <c r="H60" t="n">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>-116580</v>
+        <v>-98549</v>
       </c>
       <c r="B61" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C61" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D61" t="n">
         <v>40000</v>
       </c>
       <c r="E61" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F61" t="n">
-        <v>83324</v>
+        <v>70662</v>
       </c>
       <c r="G61" t="n">
-        <v>-33740.44719151744</v>
+        <v>-24214.27237016515</v>
       </c>
       <c r="H61" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>-102704</v>
+        <v>-106718</v>
       </c>
       <c r="B62" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C62" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="D62" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E62" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F62" t="n">
-        <v>42543</v>
+        <v>57316</v>
       </c>
       <c r="G62" t="n">
-        <v>-24272.08834649093</v>
+        <v>7644.982522217972</v>
       </c>
       <c r="H62" t="n">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>-112589</v>
+        <v>-90321</v>
       </c>
       <c r="B63" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C63" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="D63" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E63" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F63" t="n">
-        <v>70474</v>
+        <v>53565</v>
       </c>
       <c r="G63" t="n">
-        <v>-4279.047753970388</v>
+        <v>12621.17327356737</v>
       </c>
       <c r="H63" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>-90433</v>
+        <v>-101135</v>
       </c>
       <c r="B64" t="n">
         <v>40000</v>
       </c>
       <c r="C64" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D64" t="n">
         <v>30000</v>
@@ -2105,36 +2105,36 @@
         <v>30000</v>
       </c>
       <c r="F64" t="n">
-        <v>73922</v>
+        <v>53736</v>
       </c>
       <c r="G64" t="n">
-        <v>-1018.057745645632</v>
+        <v>-10132.51977126568</v>
       </c>
       <c r="H64" t="n">
-        <v>0.23</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>-96493</v>
+        <v>-83720</v>
       </c>
       <c r="B65" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C65" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D65" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E65" t="n">
         <v>60000</v>
       </c>
       <c r="F65" t="n">
-        <v>53915</v>
+        <v>59371</v>
       </c>
       <c r="G65" t="n">
-        <v>-13091.02520115151</v>
+        <v>23740.32155818752</v>
       </c>
       <c r="H65" t="n">
         <v>0.21</v>
@@ -2142,88 +2142,88 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>-92209</v>
+        <v>-109328</v>
       </c>
       <c r="B66" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C66" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D66" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E66" t="n">
         <v>30000</v>
       </c>
       <c r="F66" t="n">
-        <v>72601</v>
+        <v>55533</v>
       </c>
       <c r="G66" t="n">
-        <v>6459.416489711427</v>
+        <v>-23163.37725780952</v>
       </c>
       <c r="H66" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>-109879</v>
+        <v>-93876</v>
       </c>
       <c r="B67" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C67" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D67" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E67" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F67" t="n">
-        <v>50195</v>
+        <v>37623</v>
       </c>
       <c r="G67" t="n">
-        <v>-46873.82490360236</v>
+        <v>-23950.4210965593</v>
       </c>
       <c r="H67" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>-126568</v>
+        <v>-101861</v>
       </c>
       <c r="B68" t="n">
         <v>40000</v>
       </c>
       <c r="C68" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D68" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E68" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F68" t="n">
-        <v>69490</v>
+        <v>58308</v>
       </c>
       <c r="G68" t="n">
-        <v>-19706.79445923451</v>
+        <v>-22762.92928155001</v>
       </c>
       <c r="H68" t="n">
-        <v>0.18</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>-99872</v>
+        <v>-94222</v>
       </c>
       <c r="B69" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C69" t="n">
         <v>60000</v>
@@ -2235,88 +2235,88 @@
         <v>20000</v>
       </c>
       <c r="F69" t="n">
-        <v>80896</v>
+        <v>69181</v>
       </c>
       <c r="G69" t="n">
-        <v>2412.968471427528</v>
+        <v>4632.095602913665</v>
       </c>
       <c r="H69" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>-100826</v>
+        <v>-95880</v>
       </c>
       <c r="B70" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C70" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D70" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E70" t="n">
         <v>60000</v>
       </c>
       <c r="F70" t="n">
-        <v>62783</v>
+        <v>71163</v>
       </c>
       <c r="G70" t="n">
-        <v>-8813.431010128517</v>
+        <v>10230.4626234701</v>
       </c>
       <c r="H70" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>-105260</v>
+        <v>-95297</v>
       </c>
       <c r="B71" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C71" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D71" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E71" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="F71" t="n">
-        <v>54778</v>
+        <v>51645</v>
       </c>
       <c r="G71" t="n">
-        <v>-11877.55111661767</v>
+        <v>-20466.8982291702</v>
       </c>
       <c r="H71" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>-85675</v>
+        <v>-95001</v>
       </c>
       <c r="B72" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C72" t="n">
         <v>40000</v>
       </c>
       <c r="D72" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E72" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="F72" t="n">
-        <v>73104</v>
+        <v>78847</v>
       </c>
       <c r="G72" t="n">
-        <v>3920.105948155753</v>
+        <v>22022.63341115137</v>
       </c>
       <c r="H72" t="n">
         <v>0.17</v>
@@ -2324,25 +2324,25 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>-106635</v>
+        <v>-122670</v>
       </c>
       <c r="B73" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C73" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D73" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E73" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F73" t="n">
-        <v>72225</v>
+        <v>53187</v>
       </c>
       <c r="G73" t="n">
-        <v>-28999.34225404375</v>
+        <v>-30578.7903943109</v>
       </c>
       <c r="H73" t="n">
         <v>0.22</v>
@@ -2350,129 +2350,129 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>-103922</v>
+        <v>-102994</v>
       </c>
       <c r="B74" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C74" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D74" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E74" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F74" t="n">
-        <v>61268</v>
+        <v>71442</v>
       </c>
       <c r="G74" t="n">
-        <v>-7475.903646398294</v>
+        <v>-16546.85548993743</v>
       </c>
       <c r="H74" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>-90595</v>
+        <v>-92664</v>
       </c>
       <c r="B75" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C75" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D75" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E75" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F75" t="n">
-        <v>73777</v>
+        <v>85500</v>
       </c>
       <c r="G75" t="n">
-        <v>-647.376100351401</v>
+        <v>16159.84982086069</v>
       </c>
       <c r="H75" t="n">
-        <v>0.17</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>-106664</v>
+        <v>-92111</v>
       </c>
       <c r="B76" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C76" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D76" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E76" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F76" t="n">
-        <v>51510</v>
+        <v>51098</v>
       </c>
       <c r="G76" t="n">
-        <v>-9768.180209925551</v>
+        <v>-12151.01557008497</v>
       </c>
       <c r="H76" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>-87547</v>
+        <v>-112930</v>
       </c>
       <c r="B77" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C77" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D77" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E77" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F77" t="n">
-        <v>49711</v>
+        <v>82295</v>
       </c>
       <c r="G77" t="n">
-        <v>18274.13227345284</v>
+        <v>-29537.24224117617</v>
       </c>
       <c r="H77" t="n">
-        <v>0.17</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>-107773</v>
+        <v>-90408</v>
       </c>
       <c r="B78" t="n">
         <v>50000</v>
       </c>
       <c r="C78" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D78" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E78" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F78" t="n">
-        <v>50278</v>
+        <v>59496</v>
       </c>
       <c r="G78" t="n">
-        <v>-24609.33605991103</v>
+        <v>17826.03738565347</v>
       </c>
       <c r="H78" t="n">
         <v>0.2</v>
@@ -2480,39 +2480,39 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>-104888</v>
+        <v>-111058</v>
       </c>
       <c r="B79" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C79" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D79" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E79" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F79" t="n">
-        <v>69570</v>
+        <v>42443</v>
       </c>
       <c r="G79" t="n">
-        <v>13403.36875285022</v>
+        <v>-24086.11715609273</v>
       </c>
       <c r="H79" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>-95575</v>
+        <v>-108425</v>
       </c>
       <c r="B80" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C80" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D80" t="n">
         <v>50000</v>
@@ -2521,348 +2521,348 @@
         <v>30000</v>
       </c>
       <c r="F80" t="n">
-        <v>73729</v>
+        <v>60509</v>
       </c>
       <c r="G80" t="n">
-        <v>-24621.33633719956</v>
+        <v>695.4473677081223</v>
       </c>
       <c r="H80" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>-89737</v>
+        <v>-103354</v>
       </c>
       <c r="B81" t="n">
         <v>60000</v>
       </c>
       <c r="C81" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D81" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E81" t="n">
         <v>30000</v>
       </c>
       <c r="F81" t="n">
-        <v>52900</v>
+        <v>37814</v>
       </c>
       <c r="G81" t="n">
-        <v>7120.461037569628</v>
+        <v>-214.0353802754662</v>
       </c>
       <c r="H81" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>-96404</v>
+        <v>-91975</v>
       </c>
       <c r="B82" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C82" t="n">
         <v>40000</v>
       </c>
       <c r="D82" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E82" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F82" t="n">
-        <v>52904</v>
+        <v>40496</v>
       </c>
       <c r="G82" t="n">
-        <v>-22539.14347598832</v>
+        <v>-2218.363558214757</v>
       </c>
       <c r="H82" t="n">
-        <v>0.18</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>-103193</v>
+        <v>-97176</v>
       </c>
       <c r="B83" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C83" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D83" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E83" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F83" t="n">
-        <v>53392</v>
+        <v>72272</v>
       </c>
       <c r="G83" t="n">
-        <v>-6991.075102828398</v>
+        <v>9928.064985152359</v>
       </c>
       <c r="H83" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>-113148</v>
+        <v>-110180</v>
       </c>
       <c r="B84" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C84" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D84" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E84" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F84" t="n">
-        <v>81639</v>
+        <v>61237</v>
       </c>
       <c r="G84" t="n">
-        <v>-10635.30704709153</v>
+        <v>-20562.86138843733</v>
       </c>
       <c r="H84" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>-98623</v>
+        <v>-107173</v>
       </c>
       <c r="B85" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C85" t="n">
         <v>60000</v>
       </c>
       <c r="D85" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E85" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F85" t="n">
-        <v>62729</v>
+        <v>80484</v>
       </c>
       <c r="G85" t="n">
-        <v>17835.58804258539</v>
+        <v>20817.66778016937</v>
       </c>
       <c r="H85" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>-97138</v>
+        <v>-114155</v>
       </c>
       <c r="B86" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="C86" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D86" t="n">
         <v>40000</v>
       </c>
       <c r="E86" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F86" t="n">
-        <v>67724</v>
+        <v>58517</v>
       </c>
       <c r="G86" t="n">
-        <v>-24597.07573765503</v>
+        <v>-32961.03758464642</v>
       </c>
       <c r="H86" t="n">
-        <v>0.18</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>-98859</v>
+        <v>-105598</v>
       </c>
       <c r="B87" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C87" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D87" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E87" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F87" t="n">
-        <v>59977</v>
+        <v>49407</v>
       </c>
       <c r="G87" t="n">
-        <v>-9228.673201010861</v>
+        <v>-18869.03048790734</v>
       </c>
       <c r="H87" t="n">
-        <v>0.18</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>-100072</v>
+        <v>-95401</v>
       </c>
       <c r="B88" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C88" t="n">
         <v>20000</v>
       </c>
       <c r="D88" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E88" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F88" t="n">
-        <v>68138</v>
+        <v>38704</v>
       </c>
       <c r="G88" t="n">
-        <v>-12068.21471248298</v>
+        <v>-7407.602153799808</v>
       </c>
       <c r="H88" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>-95058</v>
+        <v>-97947</v>
       </c>
       <c r="B89" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C89" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D89" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E89" t="n">
         <v>50000</v>
       </c>
       <c r="F89" t="n">
-        <v>41743</v>
+        <v>63447</v>
       </c>
       <c r="G89" t="n">
-        <v>7809.425313460535</v>
+        <v>-4774.13025219098</v>
       </c>
       <c r="H89" t="n">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>-93681</v>
+        <v>-115962</v>
       </c>
       <c r="B90" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C90" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D90" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="E90" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F90" t="n">
-        <v>82351</v>
+        <v>50779</v>
       </c>
       <c r="G90" t="n">
-        <v>-6382.748446483231</v>
+        <v>-36559.95087905235</v>
       </c>
       <c r="H90" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>-115668</v>
+        <v>-95895</v>
       </c>
       <c r="B91" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C91" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="D91" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E91" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F91" t="n">
-        <v>83058</v>
+        <v>52663</v>
       </c>
       <c r="G91" t="n">
-        <v>-19680.01248706195</v>
+        <v>-7455.454515436189</v>
       </c>
       <c r="H91" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>-106856</v>
+        <v>-107732</v>
       </c>
       <c r="B92" t="n">
         <v>60000</v>
       </c>
       <c r="C92" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D92" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E92" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F92" t="n">
-        <v>70533</v>
+        <v>62822</v>
       </c>
       <c r="G92" t="n">
-        <v>-1384.910370611367</v>
+        <v>-10665.88991154404</v>
       </c>
       <c r="H92" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>-93257</v>
+        <v>-86668</v>
       </c>
       <c r="B93" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C93" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D93" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E93" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F93" t="n">
-        <v>57576</v>
+        <v>41768</v>
       </c>
       <c r="G93" t="n">
-        <v>16302.93791912161</v>
+        <v>-11952.72554292771</v>
       </c>
       <c r="H93" t="n">
         <v>0.2</v>
@@ -2870,85 +2870,85 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>-97538</v>
+        <v>-111601</v>
       </c>
       <c r="B94" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C94" t="n">
         <v>20000</v>
       </c>
       <c r="D94" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E94" t="n">
         <v>30000</v>
       </c>
       <c r="F94" t="n">
-        <v>58326</v>
+        <v>49469</v>
       </c>
       <c r="G94" t="n">
-        <v>-17415.45305769956</v>
+        <v>-48731.07230963479</v>
       </c>
       <c r="H94" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>-100875</v>
+        <v>-113820</v>
       </c>
       <c r="B95" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C95" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D95" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E95" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F95" t="n">
-        <v>83235</v>
+        <v>80989</v>
       </c>
       <c r="G95" t="n">
-        <v>-22221.23797718924</v>
+        <v>-11953.48670969492</v>
       </c>
       <c r="H95" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>-105038</v>
+        <v>-116845</v>
       </c>
       <c r="B96" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C96" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D96" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E96" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F96" t="n">
-        <v>48223</v>
+        <v>69667</v>
       </c>
       <c r="G96" t="n">
-        <v>2083.263427027909</v>
+        <v>-46144.72251216156</v>
       </c>
       <c r="H96" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>-100999</v>
+        <v>-103678</v>
       </c>
       <c r="B97" t="n">
         <v>40000</v>
@@ -2960,117 +2960,117 @@
         <v>60000</v>
       </c>
       <c r="E97" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="F97" t="n">
-        <v>37809</v>
+        <v>58698</v>
       </c>
       <c r="G97" t="n">
-        <v>-22357.32348273803</v>
+        <v>-30309.22711207667</v>
       </c>
       <c r="H97" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>-109767</v>
+        <v>-116108</v>
       </c>
       <c r="B98" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C98" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D98" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E98" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F98" t="n">
-        <v>61514</v>
+        <v>48149</v>
       </c>
       <c r="G98" t="n">
-        <v>-30125.22107213069</v>
+        <v>-11291.15161327942</v>
       </c>
       <c r="H98" t="n">
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>-89515</v>
+        <v>-105893</v>
       </c>
       <c r="B99" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C99" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D99" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E99" t="n">
         <v>20000</v>
       </c>
       <c r="F99" t="n">
-        <v>80532</v>
+        <v>71060</v>
       </c>
       <c r="G99" t="n">
-        <v>-2773.893614816639</v>
+        <v>-50949.02439781265</v>
       </c>
       <c r="H99" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>-119069</v>
+        <v>-116860</v>
       </c>
       <c r="B100" t="n">
         <v>60000</v>
       </c>
       <c r="C100" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="D100" t="n">
         <v>40000</v>
       </c>
       <c r="E100" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F100" t="n">
-        <v>81305</v>
+        <v>40433</v>
       </c>
       <c r="G100" t="n">
-        <v>-24418.09493913071</v>
+        <v>-17371.61974427236</v>
       </c>
       <c r="H100" t="n">
-        <v>0.18</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>-120218</v>
+        <v>-91661</v>
       </c>
       <c r="B101" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C101" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D101" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E101" t="n">
         <v>30000</v>
       </c>
       <c r="F101" t="n">
-        <v>79756</v>
+        <v>48727</v>
       </c>
       <c r="G101" t="n">
-        <v>-35629.92221485257</v>
+        <v>-16899.37988870322</v>
       </c>
       <c r="H101" t="n">
         <v>0.18</v>

</xml_diff>

<commit_message>
conclusiones escenario1 y escenario1 funcionando en los reportes
</commit_message>
<xml_diff>
--- a/escenario_2/export_dataframe.xlsx
+++ b/escenario_2/export_dataframe.xlsx
@@ -478,51 +478,51 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-111166</v>
+        <v>-114225</v>
       </c>
       <c r="B2" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C2" t="n">
         <v>60000</v>
       </c>
       <c r="D2" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E2" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F2" t="n">
-        <v>40497</v>
+        <v>38793</v>
       </c>
       <c r="G2" t="n">
-        <v>4767.321649234811</v>
+        <v>-34963.80194387468</v>
       </c>
       <c r="H2" t="n">
-        <v>0.18</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-119715</v>
+        <v>-98438</v>
       </c>
       <c r="B3" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C3" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D3" t="n">
         <v>60000</v>
       </c>
       <c r="E3" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F3" t="n">
-        <v>39628</v>
+        <v>53646</v>
       </c>
       <c r="G3" t="n">
-        <v>-41957.71296485801</v>
+        <v>-9125.241072456993</v>
       </c>
       <c r="H3" t="n">
         <v>0.21</v>
@@ -530,33 +530,33 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-100916</v>
+        <v>-94837</v>
       </c>
       <c r="B4" t="n">
         <v>30000</v>
       </c>
       <c r="C4" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D4" t="n">
         <v>30000</v>
       </c>
       <c r="E4" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F4" t="n">
-        <v>44316</v>
+        <v>80731</v>
       </c>
       <c r="G4" t="n">
-        <v>-33394.62549296932</v>
+        <v>-4230.676457607071</v>
       </c>
       <c r="H4" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-110652</v>
+        <v>-119360</v>
       </c>
       <c r="B5" t="n">
         <v>40000</v>
@@ -571,36 +571,36 @@
         <v>30000</v>
       </c>
       <c r="F5" t="n">
-        <v>60537</v>
+        <v>70643</v>
       </c>
       <c r="G5" t="n">
-        <v>-26296.25502964172</v>
+        <v>-31308.42081733626</v>
       </c>
       <c r="H5" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-97947</v>
+        <v>-85662</v>
       </c>
       <c r="B6" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C6" t="n">
         <v>30000</v>
       </c>
       <c r="D6" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E6" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F6" t="n">
-        <v>37616</v>
+        <v>68197</v>
       </c>
       <c r="G6" t="n">
-        <v>-14502.74288570416</v>
+        <v>7616.987744002474</v>
       </c>
       <c r="H6" t="n">
         <v>0.19</v>
@@ -608,65 +608,65 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-104810</v>
+        <v>-90922</v>
       </c>
       <c r="B7" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C7" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D7" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E7" t="n">
         <v>50000</v>
       </c>
       <c r="F7" t="n">
-        <v>80180</v>
+        <v>63128</v>
       </c>
       <c r="G7" t="n">
-        <v>-8007.030463158371</v>
+        <v>-11403.95789581037</v>
       </c>
       <c r="H7" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-110734</v>
+        <v>-95613</v>
       </c>
       <c r="B8" t="n">
         <v>30000</v>
       </c>
       <c r="C8" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D8" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E8" t="n">
         <v>20000</v>
       </c>
       <c r="F8" t="n">
-        <v>53548</v>
+        <v>41595</v>
       </c>
       <c r="G8" t="n">
-        <v>-35949.26114637084</v>
+        <v>-31434.28704505908</v>
       </c>
       <c r="H8" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-117473</v>
+        <v>-86329</v>
       </c>
       <c r="B9" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C9" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D9" t="n">
         <v>20000</v>
@@ -675,218 +675,218 @@
         <v>50000</v>
       </c>
       <c r="F9" t="n">
-        <v>59315</v>
+        <v>49876</v>
       </c>
       <c r="G9" t="n">
-        <v>-2820.302087770953</v>
+        <v>-11209.23160070717</v>
       </c>
       <c r="H9" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-94208</v>
+        <v>-104355</v>
       </c>
       <c r="B10" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C10" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D10" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E10" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F10" t="n">
-        <v>64284</v>
+        <v>79721</v>
       </c>
       <c r="G10" t="n">
-        <v>2348.126633903568</v>
+        <v>10717.58145911682</v>
       </c>
       <c r="H10" t="n">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-95225</v>
+        <v>-91676</v>
       </c>
       <c r="B11" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C11" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="D11" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E11" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F11" t="n">
-        <v>39125</v>
+        <v>60594</v>
       </c>
       <c r="G11" t="n">
-        <v>-6264.927099726179</v>
+        <v>-15869.72344061047</v>
       </c>
       <c r="H11" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-127066</v>
+        <v>-119143</v>
       </c>
       <c r="B12" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="C12" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D12" t="n">
         <v>40000</v>
       </c>
       <c r="E12" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F12" t="n">
-        <v>48011</v>
+        <v>69544</v>
       </c>
       <c r="G12" t="n">
-        <v>-53731.60419435684</v>
+        <v>-19226.60007925477</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-114899</v>
+        <v>-90543</v>
       </c>
       <c r="B13" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C13" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D13" t="n">
         <v>60000</v>
       </c>
       <c r="E13" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F13" t="n">
-        <v>48267</v>
+        <v>40215</v>
       </c>
       <c r="G13" t="n">
-        <v>-39394.41668189845</v>
+        <v>28775.56403377543</v>
       </c>
       <c r="H13" t="n">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-90830</v>
+        <v>-95505</v>
       </c>
       <c r="B14" t="n">
         <v>30000</v>
       </c>
       <c r="C14" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D14" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E14" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F14" t="n">
-        <v>50237</v>
+        <v>39583</v>
       </c>
       <c r="G14" t="n">
-        <v>-32367.0603710906</v>
+        <v>-10188.64396944409</v>
       </c>
       <c r="H14" t="n">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-100931</v>
+        <v>-112440</v>
       </c>
       <c r="B15" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C15" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D15" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E15" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F15" t="n">
-        <v>84852</v>
+        <v>60262</v>
       </c>
       <c r="G15" t="n">
-        <v>10957.7342711441</v>
+        <v>-27252.54108417818</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-93237</v>
+        <v>-107672</v>
       </c>
       <c r="B16" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C16" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D16" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E16" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F16" t="n">
-        <v>70357</v>
+        <v>70455</v>
       </c>
       <c r="G16" t="n">
-        <v>28714.9646919414</v>
+        <v>-13945.04579695705</v>
       </c>
       <c r="H16" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-111652</v>
+        <v>-111028</v>
       </c>
       <c r="B17" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C17" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="D17" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E17" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F17" t="n">
-        <v>59704</v>
+        <v>71013</v>
       </c>
       <c r="G17" t="n">
-        <v>-53595.10999069365</v>
+        <v>-2224.599346423945</v>
       </c>
       <c r="H17" t="n">
         <v>0.2</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-90344</v>
+        <v>-109934</v>
       </c>
       <c r="B18" t="n">
         <v>30000</v>
@@ -903,16 +903,16 @@
         <v>20000</v>
       </c>
       <c r="D18" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E18" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F18" t="n">
-        <v>44059</v>
+        <v>62888</v>
       </c>
       <c r="G18" t="n">
-        <v>-25453.58921025759</v>
+        <v>-39019.42419216949</v>
       </c>
       <c r="H18" t="n">
         <v>0.19</v>
@@ -920,25 +920,25 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-118559</v>
+        <v>-88351</v>
       </c>
       <c r="B19" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C19" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D19" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E19" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F19" t="n">
-        <v>40999</v>
+        <v>81081</v>
       </c>
       <c r="G19" t="n">
-        <v>-24407.49498253706</v>
+        <v>8821.310492631243</v>
       </c>
       <c r="H19" t="n">
         <v>0.21</v>
@@ -946,467 +946,467 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-102141</v>
+        <v>-99746</v>
       </c>
       <c r="B20" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C20" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D20" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E20" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F20" t="n">
-        <v>64775</v>
+        <v>61055</v>
       </c>
       <c r="G20" t="n">
-        <v>-16707.31080287175</v>
+        <v>-4715.316717718937</v>
       </c>
       <c r="H20" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>-100072</v>
+        <v>-103674</v>
       </c>
       <c r="B21" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C21" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D21" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E21" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F21" t="n">
-        <v>73517</v>
+        <v>42548</v>
       </c>
       <c r="G21" t="n">
-        <v>-3818.087548277781</v>
+        <v>-37841.15476875862</v>
       </c>
       <c r="H21" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>-108312</v>
+        <v>-106141</v>
       </c>
       <c r="B22" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C22" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D22" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E22" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F22" t="n">
-        <v>69940</v>
+        <v>70681</v>
       </c>
       <c r="G22" t="n">
-        <v>-29647.10330246377</v>
+        <v>-18005.6633194286</v>
       </c>
       <c r="H22" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>-124211</v>
+        <v>-102916</v>
       </c>
       <c r="B23" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C23" t="n">
         <v>40000</v>
       </c>
       <c r="D23" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E23" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="F23" t="n">
-        <v>42981</v>
+        <v>79772</v>
       </c>
       <c r="G23" t="n">
-        <v>-32031.42945585073</v>
+        <v>-11422.25750468891</v>
       </c>
       <c r="H23" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>-108723</v>
+        <v>-120302</v>
       </c>
       <c r="B24" t="n">
         <v>60000</v>
       </c>
       <c r="C24" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D24" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="E24" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F24" t="n">
-        <v>79452</v>
+        <v>84048</v>
       </c>
       <c r="G24" t="n">
-        <v>-21116.52703061449</v>
+        <v>-6161.819759000224</v>
       </c>
       <c r="H24" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>-105082</v>
+        <v>-110272</v>
       </c>
       <c r="B25" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C25" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D25" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E25" t="n">
         <v>50000</v>
       </c>
       <c r="F25" t="n">
-        <v>68442</v>
+        <v>60667</v>
       </c>
       <c r="G25" t="n">
-        <v>2497.546528830993</v>
+        <v>-8637.124851308707</v>
       </c>
       <c r="H25" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>-87094</v>
+        <v>-114595</v>
       </c>
       <c r="B26" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C26" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D26" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E26" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F26" t="n">
-        <v>81746</v>
+        <v>83500</v>
       </c>
       <c r="G26" t="n">
-        <v>25940.0510228132</v>
+        <v>-26812.76844516057</v>
       </c>
       <c r="H26" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-118292</v>
+        <v>-98538</v>
       </c>
       <c r="B27" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C27" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="D27" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E27" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F27" t="n">
-        <v>41010</v>
+        <v>39039</v>
       </c>
       <c r="G27" t="n">
-        <v>-52792.26507518956</v>
+        <v>2851.345617266158</v>
       </c>
       <c r="H27" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-108352</v>
+        <v>-91425</v>
       </c>
       <c r="B28" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C28" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D28" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E28" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F28" t="n">
-        <v>59230</v>
+        <v>79667</v>
       </c>
       <c r="G28" t="n">
-        <v>-23598.88413503208</v>
+        <v>13705.02053630245</v>
       </c>
       <c r="H28" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-102809</v>
+        <v>-105969</v>
       </c>
       <c r="B29" t="n">
         <v>60000</v>
       </c>
       <c r="C29" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D29" t="n">
         <v>50000</v>
       </c>
       <c r="E29" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F29" t="n">
-        <v>58693</v>
+        <v>82006</v>
       </c>
       <c r="G29" t="n">
-        <v>14865.17717182684</v>
+        <v>-4448.855439740166</v>
       </c>
       <c r="H29" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>-104372</v>
+        <v>-116472</v>
       </c>
       <c r="B30" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C30" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D30" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E30" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F30" t="n">
-        <v>66667</v>
+        <v>52231</v>
       </c>
       <c r="G30" t="n">
-        <v>-10419.09515386966</v>
+        <v>-31065.50691519595</v>
       </c>
       <c r="H30" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-97929</v>
+        <v>-89716</v>
       </c>
       <c r="B31" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C31" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D31" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E31" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F31" t="n">
-        <v>58123</v>
+        <v>54430</v>
       </c>
       <c r="G31" t="n">
-        <v>-13082.69107964482</v>
+        <v>-36411.90957510715</v>
       </c>
       <c r="H31" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-109635</v>
+        <v>-109160</v>
       </c>
       <c r="B32" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="C32" t="n">
         <v>50000</v>
       </c>
       <c r="D32" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E32" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F32" t="n">
-        <v>48950</v>
+        <v>72417</v>
       </c>
       <c r="G32" t="n">
-        <v>-23643.20352761883</v>
+        <v>-25608.72501105672</v>
       </c>
       <c r="H32" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-98911</v>
+        <v>-89300</v>
       </c>
       <c r="B33" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C33" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D33" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E33" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F33" t="n">
-        <v>60631</v>
+        <v>81247</v>
       </c>
       <c r="G33" t="n">
-        <v>21378.42075759919</v>
+        <v>-15504.10466128859</v>
       </c>
       <c r="H33" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-110593</v>
+        <v>-113252</v>
       </c>
       <c r="B34" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C34" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D34" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="E34" t="n">
         <v>60000</v>
       </c>
       <c r="F34" t="n">
-        <v>46839</v>
+        <v>80308</v>
       </c>
       <c r="G34" t="n">
-        <v>-5534.851727173271</v>
+        <v>-596.0403783108413</v>
       </c>
       <c r="H34" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-108244</v>
+        <v>-98911</v>
       </c>
       <c r="B35" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C35" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D35" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E35" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F35" t="n">
-        <v>80456</v>
+        <v>50691</v>
       </c>
       <c r="G35" t="n">
-        <v>-22493.44887999741</v>
+        <v>-6126.457401685804</v>
       </c>
       <c r="H35" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>-93767</v>
+        <v>-92812</v>
       </c>
       <c r="B36" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C36" t="n">
         <v>20000</v>
       </c>
       <c r="D36" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E36" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F36" t="n">
-        <v>38658</v>
+        <v>79668</v>
       </c>
       <c r="G36" t="n">
-        <v>-47776.78303859817</v>
+        <v>-14499.64687088407</v>
       </c>
       <c r="H36" t="n">
-        <v>0.25</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-101088</v>
+        <v>-93903</v>
       </c>
       <c r="B37" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C37" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D37" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E37" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F37" t="n">
-        <v>49503</v>
+        <v>64264</v>
       </c>
       <c r="G37" t="n">
-        <v>-37459.17084409539</v>
+        <v>4132.08900127553</v>
       </c>
       <c r="H37" t="n">
         <v>0.2</v>
@@ -1414,117 +1414,117 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>-122805</v>
+        <v>-106377</v>
       </c>
       <c r="B38" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="C38" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D38" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E38" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="F38" t="n">
-        <v>70852</v>
+        <v>39402</v>
       </c>
       <c r="G38" t="n">
-        <v>-44557.19283825087</v>
+        <v>-23285.62998319705</v>
       </c>
       <c r="H38" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-96925</v>
+        <v>-99670</v>
       </c>
       <c r="B39" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C39" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D39" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E39" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F39" t="n">
-        <v>64566</v>
+        <v>51955</v>
       </c>
       <c r="G39" t="n">
-        <v>-33243.70924331572</v>
+        <v>-15145.74824217923</v>
       </c>
       <c r="H39" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>-86454</v>
+        <v>-98711</v>
       </c>
       <c r="B40" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C40" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D40" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="E40" t="n">
         <v>40000</v>
       </c>
       <c r="F40" t="n">
-        <v>58354</v>
+        <v>69522</v>
       </c>
       <c r="G40" t="n">
-        <v>-12238.17081696276</v>
+        <v>1116.350538609895</v>
       </c>
       <c r="H40" t="n">
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>-114010</v>
+        <v>-104460</v>
       </c>
       <c r="B41" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C41" t="n">
         <v>30000</v>
       </c>
       <c r="D41" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E41" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F41" t="n">
-        <v>50938</v>
+        <v>59645</v>
       </c>
       <c r="G41" t="n">
-        <v>-27913.4426988749</v>
+        <v>-34679.44248765821</v>
       </c>
       <c r="H41" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>-103474</v>
+        <v>-85545</v>
       </c>
       <c r="B42" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C42" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D42" t="n">
         <v>60000</v>
@@ -1533,10 +1533,10 @@
         <v>30000</v>
       </c>
       <c r="F42" t="n">
-        <v>49929</v>
+        <v>78153</v>
       </c>
       <c r="G42" t="n">
-        <v>-28506.36288787763</v>
+        <v>4014.461320104228</v>
       </c>
       <c r="H42" t="n">
         <v>0.19</v>
@@ -1544,36 +1544,36 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>-99352</v>
+        <v>-103799</v>
       </c>
       <c r="B43" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C43" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D43" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="E43" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="F43" t="n">
-        <v>78009</v>
+        <v>80316</v>
       </c>
       <c r="G43" t="n">
-        <v>-17320.34941885038</v>
+        <v>-17997.01394274992</v>
       </c>
       <c r="H43" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>-109229</v>
+        <v>-93290</v>
       </c>
       <c r="B44" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C44" t="n">
         <v>30000</v>
@@ -1585,10 +1585,10 @@
         <v>20000</v>
       </c>
       <c r="F44" t="n">
-        <v>80907</v>
+        <v>77350</v>
       </c>
       <c r="G44" t="n">
-        <v>-31031.37047153969</v>
+        <v>5936.056497669366</v>
       </c>
       <c r="H44" t="n">
         <v>0.2</v>
@@ -1596,296 +1596,296 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>-101333</v>
+        <v>-104924</v>
       </c>
       <c r="B45" t="n">
         <v>20000</v>
       </c>
       <c r="C45" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D45" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E45" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F45" t="n">
-        <v>51257</v>
+        <v>70148</v>
       </c>
       <c r="G45" t="n">
-        <v>-30489.09608159261</v>
+        <v>-22371.93373178653</v>
       </c>
       <c r="H45" t="n">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>-92394</v>
+        <v>-88971</v>
       </c>
       <c r="B46" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C46" t="n">
         <v>20000</v>
       </c>
       <c r="D46" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E46" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F46" t="n">
-        <v>52042</v>
+        <v>70223</v>
       </c>
       <c r="G46" t="n">
-        <v>-36405.39240979103</v>
+        <v>-15886.99172545249</v>
       </c>
       <c r="H46" t="n">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>-112660</v>
+        <v>-95831</v>
       </c>
       <c r="B47" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C47" t="n">
         <v>40000</v>
       </c>
       <c r="D47" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E47" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F47" t="n">
-        <v>78449</v>
+        <v>43755</v>
       </c>
       <c r="G47" t="n">
-        <v>-16941.51929581302</v>
+        <v>-25274.52316321016</v>
       </c>
       <c r="H47" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>-102941</v>
+        <v>-94238</v>
       </c>
       <c r="B48" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C48" t="n">
         <v>30000</v>
       </c>
       <c r="D48" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E48" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="F48" t="n">
-        <v>80814</v>
+        <v>80235</v>
       </c>
       <c r="G48" t="n">
-        <v>-25118.57124298393</v>
+        <v>-11651.43997823999</v>
       </c>
       <c r="H48" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>-103655</v>
+        <v>-119778</v>
       </c>
       <c r="B49" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C49" t="n">
         <v>30000</v>
       </c>
       <c r="D49" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E49" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="F49" t="n">
-        <v>53809</v>
+        <v>71198</v>
       </c>
       <c r="G49" t="n">
-        <v>-17207.18057440033</v>
+        <v>-30075.288740598</v>
       </c>
       <c r="H49" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>-95730</v>
+        <v>-97769</v>
       </c>
       <c r="B50" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C50" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D50" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E50" t="n">
         <v>20000</v>
       </c>
       <c r="F50" t="n">
-        <v>50459</v>
+        <v>51729</v>
       </c>
       <c r="G50" t="n">
-        <v>-17997.53549233059</v>
+        <v>-27245.15295793467</v>
       </c>
       <c r="H50" t="n">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>-95992</v>
+        <v>-114710</v>
       </c>
       <c r="B51" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C51" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D51" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E51" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F51" t="n">
-        <v>40512</v>
+        <v>48518</v>
       </c>
       <c r="G51" t="n">
-        <v>6636.839722150153</v>
+        <v>-20215.82174592851</v>
       </c>
       <c r="H51" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>-98248</v>
+        <v>-103538</v>
       </c>
       <c r="B52" t="n">
         <v>20000</v>
       </c>
       <c r="C52" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D52" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E52" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F52" t="n">
-        <v>50956</v>
+        <v>80564</v>
       </c>
       <c r="G52" t="n">
-        <v>-32409.25165215396</v>
+        <v>-36240.81721095571</v>
       </c>
       <c r="H52" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>-114556</v>
+        <v>-93722</v>
       </c>
       <c r="B53" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C53" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D53" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E53" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F53" t="n">
-        <v>67747</v>
+        <v>83177</v>
       </c>
       <c r="G53" t="n">
-        <v>858.4511292104435</v>
+        <v>5099.464688578038</v>
       </c>
       <c r="H53" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>-121301</v>
+        <v>-102232</v>
       </c>
       <c r="B54" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C54" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D54" t="n">
         <v>30000</v>
       </c>
       <c r="E54" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F54" t="n">
-        <v>41007</v>
+        <v>40705</v>
       </c>
       <c r="G54" t="n">
-        <v>-69602.20771117421</v>
+        <v>-24726.27858050058</v>
       </c>
       <c r="H54" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>-98367</v>
+        <v>-115256</v>
       </c>
       <c r="B55" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C55" t="n">
         <v>50000</v>
       </c>
       <c r="D55" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E55" t="n">
         <v>20000</v>
       </c>
       <c r="F55" t="n">
-        <v>60995</v>
+        <v>40463</v>
       </c>
       <c r="G55" t="n">
-        <v>-15233.41859220002</v>
+        <v>-36225.56062979306</v>
       </c>
       <c r="H55" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>-105105</v>
+        <v>-98408</v>
       </c>
       <c r="B56" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C56" t="n">
         <v>60000</v>
@@ -1894,195 +1894,195 @@
         <v>40000</v>
       </c>
       <c r="E56" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F56" t="n">
-        <v>62242</v>
+        <v>49821</v>
       </c>
       <c r="G56" t="n">
-        <v>4399.205389714674</v>
+        <v>-20649.95271615501</v>
       </c>
       <c r="H56" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>-83190</v>
+        <v>-84710</v>
       </c>
       <c r="B57" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C57" t="n">
         <v>40000</v>
       </c>
       <c r="D57" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E57" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F57" t="n">
-        <v>39954</v>
+        <v>69583</v>
       </c>
       <c r="G57" t="n">
-        <v>9587.227544618394</v>
+        <v>-7854.951113873454</v>
       </c>
       <c r="H57" t="n">
-        <v>0.22</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>-95742</v>
+        <v>-111088</v>
       </c>
       <c r="B58" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C58" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D58" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E58" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F58" t="n">
-        <v>60508</v>
+        <v>49760</v>
       </c>
       <c r="G58" t="n">
-        <v>-35537.1929291237</v>
+        <v>-34293.48080365843</v>
       </c>
       <c r="H58" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>-105531</v>
+        <v>-109386</v>
       </c>
       <c r="B59" t="n">
         <v>60000</v>
       </c>
       <c r="C59" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D59" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E59" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F59" t="n">
-        <v>52197</v>
+        <v>38462</v>
       </c>
       <c r="G59" t="n">
-        <v>-13311.34748499166</v>
+        <v>-3689.701186961483</v>
       </c>
       <c r="H59" t="n">
-        <v>0.23</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>-120602</v>
+        <v>-122686</v>
       </c>
       <c r="B60" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C60" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D60" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E60" t="n">
         <v>50000</v>
       </c>
       <c r="F60" t="n">
-        <v>69474</v>
+        <v>82570</v>
       </c>
       <c r="G60" t="n">
-        <v>-33374.29284342394</v>
+        <v>-53809.42562419607</v>
       </c>
       <c r="H60" t="n">
-        <v>0.17</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>-98549</v>
+        <v>-109595</v>
       </c>
       <c r="B61" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C61" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="D61" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E61" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F61" t="n">
-        <v>70662</v>
+        <v>48825</v>
       </c>
       <c r="G61" t="n">
-        <v>-24214.27237016515</v>
+        <v>-6178.095393819345</v>
       </c>
       <c r="H61" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>-106718</v>
+        <v>-104072</v>
       </c>
       <c r="B62" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C62" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D62" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E62" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F62" t="n">
-        <v>57316</v>
+        <v>80280</v>
       </c>
       <c r="G62" t="n">
-        <v>7644.982522217972</v>
+        <v>-22988.77868804847</v>
       </c>
       <c r="H62" t="n">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>-90321</v>
+        <v>-107876</v>
       </c>
       <c r="B63" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C63" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D63" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E63" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F63" t="n">
-        <v>53565</v>
+        <v>60258</v>
       </c>
       <c r="G63" t="n">
-        <v>12621.17327356737</v>
+        <v>-14532.71956390169</v>
       </c>
       <c r="H63" t="n">
         <v>0.22</v>
@@ -2090,181 +2090,181 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>-101135</v>
+        <v>-102233</v>
       </c>
       <c r="B64" t="n">
         <v>40000</v>
       </c>
       <c r="C64" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D64" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E64" t="n">
         <v>30000</v>
       </c>
       <c r="F64" t="n">
-        <v>53736</v>
+        <v>38521</v>
       </c>
       <c r="G64" t="n">
-        <v>-10132.51977126568</v>
+        <v>-39166.80598600775</v>
       </c>
       <c r="H64" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>-83720</v>
+        <v>-99771</v>
       </c>
       <c r="B65" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C65" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D65" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E65" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F65" t="n">
-        <v>59371</v>
+        <v>70397</v>
       </c>
       <c r="G65" t="n">
-        <v>23740.32155818752</v>
+        <v>-22438.75428779523</v>
       </c>
       <c r="H65" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>-109328</v>
+        <v>-111525</v>
       </c>
       <c r="B66" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C66" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D66" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E66" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F66" t="n">
-        <v>55533</v>
+        <v>61855</v>
       </c>
       <c r="G66" t="n">
-        <v>-23163.37725780952</v>
+        <v>-35439.73375493419</v>
       </c>
       <c r="H66" t="n">
-        <v>0.23</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>-93876</v>
+        <v>-101415</v>
       </c>
       <c r="B67" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C67" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D67" t="n">
         <v>50000</v>
       </c>
       <c r="E67" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F67" t="n">
-        <v>37623</v>
+        <v>61397</v>
       </c>
       <c r="G67" t="n">
-        <v>-23950.4210965593</v>
+        <v>-9367.177817888465</v>
       </c>
       <c r="H67" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>-101861</v>
+        <v>-85190</v>
       </c>
       <c r="B68" t="n">
         <v>40000</v>
       </c>
       <c r="C68" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D68" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E68" t="n">
         <v>40000</v>
       </c>
       <c r="F68" t="n">
-        <v>58308</v>
+        <v>40002</v>
       </c>
       <c r="G68" t="n">
-        <v>-22762.92928155001</v>
+        <v>13348.60480388621</v>
       </c>
       <c r="H68" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>-94222</v>
+        <v>-104133</v>
       </c>
       <c r="B69" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C69" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D69" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E69" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F69" t="n">
-        <v>69181</v>
+        <v>84149</v>
       </c>
       <c r="G69" t="n">
-        <v>4632.095602913665</v>
+        <v>-45208.8497139291</v>
       </c>
       <c r="H69" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>-95880</v>
+        <v>-97956</v>
       </c>
       <c r="B70" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C70" t="n">
         <v>60000</v>
       </c>
       <c r="D70" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E70" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F70" t="n">
-        <v>71163</v>
+        <v>61799</v>
       </c>
       <c r="G70" t="n">
-        <v>10230.4626234701</v>
+        <v>84.89259338754709</v>
       </c>
       <c r="H70" t="n">
         <v>0.2</v>
@@ -2272,25 +2272,25 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>-95297</v>
+        <v>-102257</v>
       </c>
       <c r="B71" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C71" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D71" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E71" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F71" t="n">
-        <v>51645</v>
+        <v>62765</v>
       </c>
       <c r="G71" t="n">
-        <v>-20466.8982291702</v>
+        <v>-22038.09805707802</v>
       </c>
       <c r="H71" t="n">
         <v>0.22</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>-95001</v>
+        <v>-94525</v>
       </c>
       <c r="B72" t="n">
         <v>50000</v>
@@ -2307,79 +2307,79 @@
         <v>40000</v>
       </c>
       <c r="D72" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E72" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="F72" t="n">
-        <v>78847</v>
+        <v>80007</v>
       </c>
       <c r="G72" t="n">
-        <v>22022.63341115137</v>
+        <v>-3604.302928390087</v>
       </c>
       <c r="H72" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>-122670</v>
+        <v>-107652</v>
       </c>
       <c r="B73" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C73" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D73" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E73" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F73" t="n">
-        <v>53187</v>
+        <v>81299</v>
       </c>
       <c r="G73" t="n">
-        <v>-30578.7903943109</v>
+        <v>-29112.44957568174</v>
       </c>
       <c r="H73" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>-102994</v>
+        <v>-86743</v>
       </c>
       <c r="B74" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="C74" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D74" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E74" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F74" t="n">
-        <v>71442</v>
+        <v>72662</v>
       </c>
       <c r="G74" t="n">
-        <v>-16546.85548993743</v>
+        <v>20637.8699335292</v>
       </c>
       <c r="H74" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>-92664</v>
+        <v>-99787</v>
       </c>
       <c r="B75" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C75" t="n">
         <v>60000</v>
@@ -2391,10 +2391,10 @@
         <v>40000</v>
       </c>
       <c r="F75" t="n">
-        <v>85500</v>
+        <v>44801</v>
       </c>
       <c r="G75" t="n">
-        <v>16159.84982086069</v>
+        <v>-5950.952261871336</v>
       </c>
       <c r="H75" t="n">
         <v>0.21</v>
@@ -2402,143 +2402,143 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>-92111</v>
+        <v>-103872</v>
       </c>
       <c r="B76" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C76" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D76" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E76" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F76" t="n">
-        <v>51098</v>
+        <v>70082</v>
       </c>
       <c r="G76" t="n">
-        <v>-12151.01557008497</v>
+        <v>-12475.1461282523</v>
       </c>
       <c r="H76" t="n">
-        <v>0.23</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>-112930</v>
+        <v>-111502</v>
       </c>
       <c r="B77" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C77" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D77" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E77" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F77" t="n">
-        <v>82295</v>
+        <v>45605</v>
       </c>
       <c r="G77" t="n">
-        <v>-29537.24224117617</v>
+        <v>-7524.752614985196</v>
       </c>
       <c r="H77" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>-90408</v>
+        <v>-85191</v>
       </c>
       <c r="B78" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C78" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D78" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E78" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F78" t="n">
-        <v>59496</v>
+        <v>72883</v>
       </c>
       <c r="G78" t="n">
-        <v>17826.03738565347</v>
+        <v>10637.778293424</v>
       </c>
       <c r="H78" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>-111058</v>
+        <v>-95328</v>
       </c>
       <c r="B79" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C79" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D79" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E79" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F79" t="n">
-        <v>42443</v>
+        <v>70415</v>
       </c>
       <c r="G79" t="n">
-        <v>-24086.11715609273</v>
+        <v>-4347.909407562793</v>
       </c>
       <c r="H79" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>-108425</v>
+        <v>-99296</v>
       </c>
       <c r="B80" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C80" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D80" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E80" t="n">
         <v>30000</v>
       </c>
       <c r="F80" t="n">
-        <v>60509</v>
+        <v>54544</v>
       </c>
       <c r="G80" t="n">
-        <v>695.4473677081223</v>
+        <v>-30961.75915908266</v>
       </c>
       <c r="H80" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>-103354</v>
+        <v>-93053</v>
       </c>
       <c r="B81" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C81" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D81" t="n">
         <v>60000</v>
@@ -2547,114 +2547,114 @@
         <v>30000</v>
       </c>
       <c r="F81" t="n">
-        <v>37814</v>
+        <v>70103</v>
       </c>
       <c r="G81" t="n">
-        <v>-214.0353802754662</v>
+        <v>-9148.782541272203</v>
       </c>
       <c r="H81" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>-91975</v>
+        <v>-117936</v>
       </c>
       <c r="B82" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C82" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D82" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E82" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F82" t="n">
-        <v>40496</v>
+        <v>82948</v>
       </c>
       <c r="G82" t="n">
-        <v>-2218.363558214757</v>
+        <v>-44809.74190874083</v>
       </c>
       <c r="H82" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>-97176</v>
+        <v>-99031</v>
       </c>
       <c r="B83" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C83" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D83" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E83" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F83" t="n">
-        <v>72272</v>
+        <v>49880</v>
       </c>
       <c r="G83" t="n">
-        <v>9928.064985152359</v>
+        <v>-12826.4106962239</v>
       </c>
       <c r="H83" t="n">
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>-110180</v>
+        <v>-104118</v>
       </c>
       <c r="B84" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C84" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D84" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E84" t="n">
         <v>30000</v>
       </c>
       <c r="F84" t="n">
-        <v>61237</v>
+        <v>79696</v>
       </c>
       <c r="G84" t="n">
-        <v>-20562.86138843733</v>
+        <v>-14804.16529652924</v>
       </c>
       <c r="H84" t="n">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>-107173</v>
+        <v>-119901</v>
       </c>
       <c r="B85" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C85" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D85" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E85" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F85" t="n">
-        <v>80484</v>
+        <v>77882</v>
       </c>
       <c r="G85" t="n">
-        <v>20817.66778016937</v>
+        <v>-17022.39878298615</v>
       </c>
       <c r="H85" t="n">
         <v>0.18</v>
@@ -2662,59 +2662,59 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>-114155</v>
+        <v>-96642</v>
       </c>
       <c r="B86" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C86" t="n">
         <v>50000</v>
       </c>
       <c r="D86" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E86" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F86" t="n">
-        <v>58517</v>
+        <v>40780</v>
       </c>
       <c r="G86" t="n">
-        <v>-32961.03758464642</v>
+        <v>17856.1768520805</v>
       </c>
       <c r="H86" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>-105598</v>
+        <v>-108671</v>
       </c>
       <c r="B87" t="n">
         <v>60000</v>
       </c>
       <c r="C87" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D87" t="n">
         <v>30000</v>
       </c>
       <c r="E87" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F87" t="n">
-        <v>49407</v>
+        <v>85111</v>
       </c>
       <c r="G87" t="n">
-        <v>-18869.03048790734</v>
+        <v>-5477.851372936781</v>
       </c>
       <c r="H87" t="n">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>-95401</v>
+        <v>-92015</v>
       </c>
       <c r="B88" t="n">
         <v>50000</v>
@@ -2723,357 +2723,357 @@
         <v>20000</v>
       </c>
       <c r="D88" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E88" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F88" t="n">
-        <v>38704</v>
+        <v>39866</v>
       </c>
       <c r="G88" t="n">
-        <v>-7407.602153799808</v>
+        <v>-12408.97367797419</v>
       </c>
       <c r="H88" t="n">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>-97947</v>
+        <v>-93310</v>
       </c>
       <c r="B89" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C89" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D89" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E89" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F89" t="n">
-        <v>63447</v>
+        <v>78654</v>
       </c>
       <c r="G89" t="n">
-        <v>-4774.13025219098</v>
+        <v>-5562.259564705952</v>
       </c>
       <c r="H89" t="n">
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>-115962</v>
+        <v>-101322</v>
       </c>
       <c r="B90" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C90" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="D90" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E90" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F90" t="n">
-        <v>50779</v>
+        <v>82433</v>
       </c>
       <c r="G90" t="n">
-        <v>-36559.95087905235</v>
+        <v>-29329.21262675518</v>
       </c>
       <c r="H90" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>-95895</v>
+        <v>-122992</v>
       </c>
       <c r="B91" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C91" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D91" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E91" t="n">
         <v>20000</v>
       </c>
       <c r="F91" t="n">
-        <v>52663</v>
+        <v>40297</v>
       </c>
       <c r="G91" t="n">
-        <v>-7455.454515436189</v>
+        <v>-47868.62560060346</v>
       </c>
       <c r="H91" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>-107732</v>
+        <v>-123334</v>
       </c>
       <c r="B92" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C92" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D92" t="n">
         <v>20000</v>
       </c>
       <c r="E92" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F92" t="n">
-        <v>62822</v>
+        <v>79453</v>
       </c>
       <c r="G92" t="n">
-        <v>-10665.88991154404</v>
+        <v>-36315.94691578385</v>
       </c>
       <c r="H92" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>-86668</v>
+        <v>-101638</v>
       </c>
       <c r="B93" t="n">
         <v>30000</v>
       </c>
       <c r="C93" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D93" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E93" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F93" t="n">
-        <v>41768</v>
+        <v>57987</v>
       </c>
       <c r="G93" t="n">
-        <v>-11952.72554292771</v>
+        <v>-14636.90119827544</v>
       </c>
       <c r="H93" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>-111601</v>
+        <v>-106539</v>
       </c>
       <c r="B94" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C94" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D94" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E94" t="n">
         <v>30000</v>
       </c>
       <c r="F94" t="n">
-        <v>49469</v>
+        <v>42724</v>
       </c>
       <c r="G94" t="n">
-        <v>-48731.07230963479</v>
+        <v>-13118.30207536499</v>
       </c>
       <c r="H94" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>-113820</v>
+        <v>-120448</v>
       </c>
       <c r="B95" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C95" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D95" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E95" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F95" t="n">
-        <v>80989</v>
+        <v>39760</v>
       </c>
       <c r="G95" t="n">
-        <v>-11953.48670969492</v>
+        <v>-55079.4924621531</v>
       </c>
       <c r="H95" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>-116845</v>
+        <v>-102642</v>
       </c>
       <c r="B96" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C96" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D96" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="E96" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F96" t="n">
-        <v>69667</v>
+        <v>41874</v>
       </c>
       <c r="G96" t="n">
-        <v>-46144.72251216156</v>
+        <v>-2019.837214949564</v>
       </c>
       <c r="H96" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>-103678</v>
+        <v>-108153</v>
       </c>
       <c r="B97" t="n">
         <v>40000</v>
       </c>
       <c r="C97" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D97" t="n">
         <v>60000</v>
       </c>
       <c r="E97" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F97" t="n">
-        <v>58698</v>
+        <v>71732</v>
       </c>
       <c r="G97" t="n">
-        <v>-30309.22711207667</v>
+        <v>-11495.85569376033</v>
       </c>
       <c r="H97" t="n">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>-116108</v>
+        <v>-98662</v>
       </c>
       <c r="B98" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C98" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D98" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E98" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F98" t="n">
-        <v>48149</v>
+        <v>43165</v>
       </c>
       <c r="G98" t="n">
-        <v>-11291.15161327942</v>
+        <v>-43065.62157124485</v>
       </c>
       <c r="H98" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>-105893</v>
+        <v>-104271</v>
       </c>
       <c r="B99" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C99" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D99" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E99" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F99" t="n">
-        <v>71060</v>
+        <v>41432</v>
       </c>
       <c r="G99" t="n">
-        <v>-50949.02439781265</v>
+        <v>-4303.062048524102</v>
       </c>
       <c r="H99" t="n">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>-116860</v>
+        <v>-107087</v>
       </c>
       <c r="B100" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C100" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D100" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E100" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F100" t="n">
-        <v>40433</v>
+        <v>40910</v>
       </c>
       <c r="G100" t="n">
-        <v>-17371.61974427236</v>
+        <v>-41777.53063166965</v>
       </c>
       <c r="H100" t="n">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>-91661</v>
+        <v>-96622</v>
       </c>
       <c r="B101" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C101" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D101" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E101" t="n">
         <v>30000</v>
       </c>
       <c r="F101" t="n">
-        <v>48727</v>
+        <v>59902</v>
       </c>
       <c r="G101" t="n">
-        <v>-16899.37988870322</v>
+        <v>-17868.5804609649</v>
       </c>
       <c r="H101" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ruta convertidor de pdf  funcionando dinamicamente
</commit_message>
<xml_diff>
--- a/escenario_2/export_dataframe.xlsx
+++ b/escenario_2/export_dataframe.xlsx
@@ -478,77 +478,77 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-114225</v>
+        <v>-116824</v>
       </c>
       <c r="B2" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C2" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D2" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E2" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F2" t="n">
-        <v>38793</v>
+        <v>53015</v>
       </c>
       <c r="G2" t="n">
-        <v>-34963.80194387468</v>
+        <v>-37338.95350174082</v>
       </c>
       <c r="H2" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-98438</v>
+        <v>-94993</v>
       </c>
       <c r="B3" t="n">
         <v>50000</v>
       </c>
       <c r="C3" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D3" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E3" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F3" t="n">
-        <v>53646</v>
+        <v>49948</v>
       </c>
       <c r="G3" t="n">
-        <v>-9125.241072456993</v>
+        <v>-14158.80317912782</v>
       </c>
       <c r="H3" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-94837</v>
+        <v>-126378</v>
       </c>
       <c r="B4" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C4" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D4" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="E4" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F4" t="n">
-        <v>80731</v>
+        <v>73568</v>
       </c>
       <c r="G4" t="n">
-        <v>-4230.676457607071</v>
+        <v>-733.7463620599501</v>
       </c>
       <c r="H4" t="n">
         <v>0.18</v>
@@ -556,519 +556,519 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-119360</v>
+        <v>-105721</v>
       </c>
       <c r="B5" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C5" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D5" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E5" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F5" t="n">
-        <v>70643</v>
+        <v>49562</v>
       </c>
       <c r="G5" t="n">
-        <v>-31308.42081733626</v>
+        <v>-18354.06655318751</v>
       </c>
       <c r="H5" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-85662</v>
+        <v>-120810</v>
       </c>
       <c r="B6" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C6" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D6" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E6" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F6" t="n">
-        <v>68197</v>
+        <v>51443</v>
       </c>
       <c r="G6" t="n">
-        <v>7616.987744002474</v>
+        <v>-49447.04373741605</v>
       </c>
       <c r="H6" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-90922</v>
+        <v>-87667</v>
       </c>
       <c r="B7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C7" t="n">
         <v>20000</v>
       </c>
       <c r="D7" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E7" t="n">
         <v>50000</v>
       </c>
       <c r="F7" t="n">
-        <v>63128</v>
+        <v>60055</v>
       </c>
       <c r="G7" t="n">
-        <v>-11403.95789581037</v>
+        <v>-14056.09790803686</v>
       </c>
       <c r="H7" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-95613</v>
+        <v>-117087</v>
       </c>
       <c r="B8" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="C8" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D8" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E8" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F8" t="n">
-        <v>41595</v>
+        <v>81835</v>
       </c>
       <c r="G8" t="n">
-        <v>-31434.28704505908</v>
+        <v>-14937.94252260896</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-86329</v>
+        <v>-86431</v>
       </c>
       <c r="B9" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C9" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D9" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E9" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="F9" t="n">
-        <v>49876</v>
+        <v>80434</v>
       </c>
       <c r="G9" t="n">
-        <v>-11209.23160070717</v>
+        <v>27493.15088449523</v>
       </c>
       <c r="H9" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-104355</v>
+        <v>-115882</v>
       </c>
       <c r="B10" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C10" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D10" t="n">
         <v>40000</v>
       </c>
       <c r="E10" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="F10" t="n">
-        <v>79721</v>
+        <v>77408</v>
       </c>
       <c r="G10" t="n">
-        <v>10717.58145911682</v>
+        <v>-41924.95842666001</v>
       </c>
       <c r="H10" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-91676</v>
+        <v>-100905</v>
       </c>
       <c r="B11" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C11" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D11" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E11" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F11" t="n">
-        <v>60594</v>
+        <v>39301</v>
       </c>
       <c r="G11" t="n">
-        <v>-15869.72344061047</v>
+        <v>-33112.31794809821</v>
       </c>
       <c r="H11" t="n">
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-119143</v>
+        <v>-98484</v>
       </c>
       <c r="B12" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C12" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D12" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E12" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F12" t="n">
-        <v>69544</v>
+        <v>84495</v>
       </c>
       <c r="G12" t="n">
-        <v>-19226.60007925477</v>
+        <v>20460.31827141636</v>
       </c>
       <c r="H12" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-90543</v>
+        <v>-94215</v>
       </c>
       <c r="B13" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C13" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D13" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E13" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F13" t="n">
-        <v>40215</v>
+        <v>59500</v>
       </c>
       <c r="G13" t="n">
-        <v>28775.56403377543</v>
+        <v>-3144.694349751784</v>
       </c>
       <c r="H13" t="n">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-95505</v>
+        <v>-121751</v>
       </c>
       <c r="B14" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C14" t="n">
         <v>60000</v>
       </c>
       <c r="D14" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E14" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F14" t="n">
-        <v>39583</v>
+        <v>61198</v>
       </c>
       <c r="G14" t="n">
-        <v>-10188.64396944409</v>
+        <v>-18526.32915939583</v>
       </c>
       <c r="H14" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-112440</v>
+        <v>-97372</v>
       </c>
       <c r="B15" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C15" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D15" t="n">
         <v>50000</v>
       </c>
       <c r="E15" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F15" t="n">
-        <v>60262</v>
+        <v>60373</v>
       </c>
       <c r="G15" t="n">
-        <v>-27252.54108417818</v>
+        <v>-22515.23093660698</v>
       </c>
       <c r="H15" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-107672</v>
+        <v>-100269</v>
       </c>
       <c r="B16" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C16" t="n">
         <v>40000</v>
       </c>
       <c r="D16" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E16" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="F16" t="n">
-        <v>70455</v>
+        <v>48399</v>
       </c>
       <c r="G16" t="n">
-        <v>-13945.04579695705</v>
+        <v>-25581.61723401055</v>
       </c>
       <c r="H16" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-111028</v>
+        <v>-96312</v>
       </c>
       <c r="B17" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C17" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D17" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E17" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F17" t="n">
-        <v>71013</v>
+        <v>79771</v>
       </c>
       <c r="G17" t="n">
-        <v>-2224.599346423945</v>
+        <v>6648.025996116254</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-109934</v>
+        <v>-99129</v>
       </c>
       <c r="B18" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C18" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D18" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E18" t="n">
         <v>20000</v>
       </c>
       <c r="F18" t="n">
-        <v>62888</v>
+        <v>70674</v>
       </c>
       <c r="G18" t="n">
-        <v>-39019.42419216949</v>
+        <v>-15718.17313591108</v>
       </c>
       <c r="H18" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-88351</v>
+        <v>-104031</v>
       </c>
       <c r="B19" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C19" t="n">
         <v>20000</v>
       </c>
       <c r="D19" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E19" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="F19" t="n">
-        <v>81081</v>
+        <v>63273</v>
       </c>
       <c r="G19" t="n">
-        <v>8821.310492631243</v>
+        <v>-32952.29887139043</v>
       </c>
       <c r="H19" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-99746</v>
+        <v>-97398</v>
       </c>
       <c r="B20" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C20" t="n">
         <v>60000</v>
       </c>
       <c r="D20" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E20" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F20" t="n">
-        <v>61055</v>
+        <v>41011</v>
       </c>
       <c r="G20" t="n">
-        <v>-4715.316717718937</v>
+        <v>-11418.76493800508</v>
       </c>
       <c r="H20" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>-103674</v>
+        <v>-106281</v>
       </c>
       <c r="B21" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C21" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D21" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E21" t="n">
         <v>60000</v>
       </c>
       <c r="F21" t="n">
-        <v>42548</v>
+        <v>72795</v>
       </c>
       <c r="G21" t="n">
-        <v>-37841.15476875862</v>
+        <v>10512.94644133991</v>
       </c>
       <c r="H21" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>-106141</v>
+        <v>-117319</v>
       </c>
       <c r="B22" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C22" t="n">
         <v>60000</v>
       </c>
       <c r="D22" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E22" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F22" t="n">
-        <v>70681</v>
+        <v>59297</v>
       </c>
       <c r="G22" t="n">
-        <v>-18005.6633194286</v>
+        <v>-6631.02363003274</v>
       </c>
       <c r="H22" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>-102916</v>
+        <v>-101005</v>
       </c>
       <c r="B23" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C23" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D23" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E23" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F23" t="n">
-        <v>79772</v>
+        <v>41003</v>
       </c>
       <c r="G23" t="n">
-        <v>-11422.25750468891</v>
+        <v>-17332.28376206204</v>
       </c>
       <c r="H23" t="n">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>-120302</v>
+        <v>-119460</v>
       </c>
       <c r="B24" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C24" t="n">
         <v>60000</v>
       </c>
       <c r="D24" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E24" t="n">
         <v>60000</v>
       </c>
       <c r="F24" t="n">
-        <v>84048</v>
+        <v>39795</v>
       </c>
       <c r="G24" t="n">
-        <v>-6161.819759000224</v>
+        <v>-37311.17991795165</v>
       </c>
       <c r="H24" t="n">
         <v>0.24</v>
@@ -1076,545 +1076,545 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>-110272</v>
+        <v>-111806</v>
       </c>
       <c r="B25" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="C25" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D25" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E25" t="n">
         <v>50000</v>
       </c>
       <c r="F25" t="n">
-        <v>60667</v>
+        <v>84051</v>
       </c>
       <c r="G25" t="n">
-        <v>-8637.124851308707</v>
+        <v>-27616.88922278371</v>
       </c>
       <c r="H25" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>-114595</v>
+        <v>-119417</v>
       </c>
       <c r="B26" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C26" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D26" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E26" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F26" t="n">
-        <v>83500</v>
+        <v>68487</v>
       </c>
       <c r="G26" t="n">
-        <v>-26812.76844516057</v>
+        <v>-38457.8174832868</v>
       </c>
       <c r="H26" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-98538</v>
+        <v>-102776</v>
       </c>
       <c r="B27" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C27" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D27" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E27" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F27" t="n">
-        <v>39039</v>
+        <v>80143</v>
       </c>
       <c r="G27" t="n">
-        <v>2851.345617266158</v>
+        <v>-35366.30225228448</v>
       </c>
       <c r="H27" t="n">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-91425</v>
+        <v>-90275</v>
       </c>
       <c r="B28" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C28" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D28" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E28" t="n">
         <v>50000</v>
       </c>
       <c r="F28" t="n">
-        <v>79667</v>
+        <v>41071</v>
       </c>
       <c r="G28" t="n">
-        <v>13705.02053630245</v>
+        <v>-147.5494550706317</v>
       </c>
       <c r="H28" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-105969</v>
+        <v>-123131</v>
       </c>
       <c r="B29" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C29" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D29" t="n">
         <v>50000</v>
       </c>
       <c r="E29" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F29" t="n">
-        <v>82006</v>
+        <v>68205</v>
       </c>
       <c r="G29" t="n">
-        <v>-4448.855439740166</v>
+        <v>-37226.50578849747</v>
       </c>
       <c r="H29" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>-116472</v>
+        <v>-91435</v>
       </c>
       <c r="B30" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="C30" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D30" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E30" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F30" t="n">
-        <v>52231</v>
+        <v>59791</v>
       </c>
       <c r="G30" t="n">
-        <v>-31065.50691519595</v>
+        <v>-14799.30495677998</v>
       </c>
       <c r="H30" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-89716</v>
+        <v>-118615</v>
       </c>
       <c r="B31" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C31" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D31" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E31" t="n">
         <v>50000</v>
       </c>
       <c r="F31" t="n">
-        <v>54430</v>
+        <v>72572</v>
       </c>
       <c r="G31" t="n">
-        <v>-36411.90957510715</v>
+        <v>-35757.11895667571</v>
       </c>
       <c r="H31" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-109160</v>
+        <v>-115036</v>
       </c>
       <c r="B32" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C32" t="n">
         <v>50000</v>
       </c>
       <c r="D32" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E32" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F32" t="n">
-        <v>72417</v>
+        <v>39507</v>
       </c>
       <c r="G32" t="n">
-        <v>-25608.72501105672</v>
+        <v>-36062.61765055125</v>
       </c>
       <c r="H32" t="n">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-89300</v>
+        <v>-102592</v>
       </c>
       <c r="B33" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C33" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D33" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E33" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F33" t="n">
-        <v>81247</v>
+        <v>56504</v>
       </c>
       <c r="G33" t="n">
-        <v>-15504.10466128859</v>
+        <v>-22859.12183247931</v>
       </c>
       <c r="H33" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-113252</v>
+        <v>-117989</v>
       </c>
       <c r="B34" t="n">
         <v>50000</v>
       </c>
       <c r="C34" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D34" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E34" t="n">
         <v>60000</v>
       </c>
       <c r="F34" t="n">
-        <v>80308</v>
+        <v>61479</v>
       </c>
       <c r="G34" t="n">
-        <v>-596.0403783108413</v>
+        <v>-15858.04448162646</v>
       </c>
       <c r="H34" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-98911</v>
+        <v>-107673</v>
       </c>
       <c r="B35" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C35" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D35" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E35" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F35" t="n">
-        <v>50691</v>
+        <v>68529</v>
       </c>
       <c r="G35" t="n">
-        <v>-6126.457401685804</v>
+        <v>-1937.523146716007</v>
       </c>
       <c r="H35" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>-92812</v>
+        <v>-97222</v>
       </c>
       <c r="B36" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C36" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="D36" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E36" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F36" t="n">
-        <v>79668</v>
+        <v>63490</v>
       </c>
       <c r="G36" t="n">
-        <v>-14499.64687088407</v>
+        <v>-6773.623699583506</v>
       </c>
       <c r="H36" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-93903</v>
+        <v>-124165</v>
       </c>
       <c r="B37" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C37" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D37" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="E37" t="n">
         <v>60000</v>
       </c>
       <c r="F37" t="n">
-        <v>64264</v>
+        <v>43979</v>
       </c>
       <c r="G37" t="n">
-        <v>4132.08900127553</v>
+        <v>-34126.947916823</v>
       </c>
       <c r="H37" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>-106377</v>
+        <v>-108023</v>
       </c>
       <c r="B38" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C38" t="n">
         <v>20000</v>
       </c>
       <c r="D38" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E38" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F38" t="n">
-        <v>39402</v>
+        <v>70541</v>
       </c>
       <c r="G38" t="n">
-        <v>-23285.62998319705</v>
+        <v>-26098.9005364401</v>
       </c>
       <c r="H38" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-99670</v>
+        <v>-121383</v>
       </c>
       <c r="B39" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C39" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D39" t="n">
         <v>20000</v>
       </c>
       <c r="E39" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F39" t="n">
-        <v>51955</v>
+        <v>78037</v>
       </c>
       <c r="G39" t="n">
-        <v>-15145.74824217923</v>
+        <v>-7183.91448342771</v>
       </c>
       <c r="H39" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>-98711</v>
+        <v>-115314</v>
       </c>
       <c r="B40" t="n">
         <v>50000</v>
       </c>
       <c r="C40" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="D40" t="n">
         <v>40000</v>
       </c>
       <c r="E40" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F40" t="n">
-        <v>69522</v>
+        <v>49555</v>
       </c>
       <c r="G40" t="n">
-        <v>1116.350538609895</v>
+        <v>-12275.04791576344</v>
       </c>
       <c r="H40" t="n">
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>-104460</v>
+        <v>-100433</v>
       </c>
       <c r="B41" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C41" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D41" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E41" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F41" t="n">
-        <v>59645</v>
+        <v>51882</v>
       </c>
       <c r="G41" t="n">
-        <v>-34679.44248765821</v>
+        <v>-3136.659543512857</v>
       </c>
       <c r="H41" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>-85545</v>
+        <v>-105487</v>
       </c>
       <c r="B42" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C42" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D42" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E42" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F42" t="n">
-        <v>78153</v>
+        <v>77712</v>
       </c>
       <c r="G42" t="n">
-        <v>4014.461320104228</v>
+        <v>-24360.42873332314</v>
       </c>
       <c r="H42" t="n">
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>-103799</v>
+        <v>-95367</v>
       </c>
       <c r="B43" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C43" t="n">
         <v>50000</v>
       </c>
       <c r="D43" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E43" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="F43" t="n">
-        <v>80316</v>
+        <v>42688</v>
       </c>
       <c r="G43" t="n">
-        <v>-17997.01394274992</v>
+        <v>-17353.19383451492</v>
       </c>
       <c r="H43" t="n">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>-93290</v>
+        <v>-93737</v>
       </c>
       <c r="B44" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C44" t="n">
         <v>30000</v>
       </c>
       <c r="D44" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E44" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F44" t="n">
-        <v>77350</v>
+        <v>61189</v>
       </c>
       <c r="G44" t="n">
-        <v>5936.056497669366</v>
+        <v>-14871.21651154755</v>
       </c>
       <c r="H44" t="n">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>-104924</v>
+        <v>-101224</v>
       </c>
       <c r="B45" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C45" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D45" t="n">
         <v>60000</v>
       </c>
       <c r="E45" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F45" t="n">
-        <v>70148</v>
+        <v>63654</v>
       </c>
       <c r="G45" t="n">
-        <v>-22371.93373178653</v>
+        <v>-10229.16754828987</v>
       </c>
       <c r="H45" t="n">
         <v>0.19</v>
@@ -1622,299 +1622,299 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>-88971</v>
+        <v>-107286</v>
       </c>
       <c r="B46" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C46" t="n">
         <v>20000</v>
       </c>
       <c r="D46" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E46" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F46" t="n">
-        <v>70223</v>
+        <v>49913</v>
       </c>
       <c r="G46" t="n">
-        <v>-15886.99172545249</v>
+        <v>-13055.49587590986</v>
       </c>
       <c r="H46" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>-95831</v>
+        <v>-105826</v>
       </c>
       <c r="B47" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C47" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D47" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E47" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F47" t="n">
-        <v>43755</v>
+        <v>72652</v>
       </c>
       <c r="G47" t="n">
-        <v>-25274.52316321016</v>
+        <v>-36630.01633262902</v>
       </c>
       <c r="H47" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>-94238</v>
+        <v>-118294</v>
       </c>
       <c r="B48" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="C48" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D48" t="n">
         <v>30000</v>
       </c>
       <c r="E48" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="F48" t="n">
-        <v>80235</v>
+        <v>81564</v>
       </c>
       <c r="G48" t="n">
-        <v>-11651.43997823999</v>
+        <v>-41133.62160750844</v>
       </c>
       <c r="H48" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>-119778</v>
+        <v>-90657</v>
       </c>
       <c r="B49" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C49" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D49" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E49" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F49" t="n">
-        <v>71198</v>
+        <v>44011</v>
       </c>
       <c r="G49" t="n">
-        <v>-30075.288740598</v>
+        <v>-7266.954804690804</v>
       </c>
       <c r="H49" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>-97769</v>
+        <v>-102068</v>
       </c>
       <c r="B50" t="n">
         <v>20000</v>
       </c>
       <c r="C50" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D50" t="n">
         <v>60000</v>
       </c>
       <c r="E50" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F50" t="n">
-        <v>51729</v>
+        <v>60428</v>
       </c>
       <c r="G50" t="n">
-        <v>-27245.15295793467</v>
+        <v>-35512.00602436814</v>
       </c>
       <c r="H50" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>-114710</v>
+        <v>-87586</v>
       </c>
       <c r="B51" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C51" t="n">
         <v>20000</v>
       </c>
       <c r="D51" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E51" t="n">
         <v>50000</v>
       </c>
       <c r="F51" t="n">
-        <v>48518</v>
+        <v>61627</v>
       </c>
       <c r="G51" t="n">
-        <v>-20215.82174592851</v>
+        <v>-11106.49656911684</v>
       </c>
       <c r="H51" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>-103538</v>
+        <v>-90992</v>
       </c>
       <c r="B52" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C52" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="D52" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E52" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F52" t="n">
-        <v>80564</v>
+        <v>51443</v>
       </c>
       <c r="G52" t="n">
-        <v>-36240.81721095571</v>
+        <v>-13045.61298066772</v>
       </c>
       <c r="H52" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>-93722</v>
+        <v>-93695</v>
       </c>
       <c r="B53" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C53" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D53" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E53" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F53" t="n">
-        <v>83177</v>
+        <v>44905</v>
       </c>
       <c r="G53" t="n">
-        <v>5099.464688578038</v>
+        <v>-12443.62112039358</v>
       </c>
       <c r="H53" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>-102232</v>
+        <v>-106969</v>
       </c>
       <c r="B54" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C54" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D54" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E54" t="n">
         <v>40000</v>
       </c>
       <c r="F54" t="n">
-        <v>40705</v>
+        <v>69932</v>
       </c>
       <c r="G54" t="n">
-        <v>-24726.27858050058</v>
+        <v>-27623.08242657928</v>
       </c>
       <c r="H54" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>-115256</v>
+        <v>-107121</v>
       </c>
       <c r="B55" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C55" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D55" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="E55" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F55" t="n">
-        <v>40463</v>
+        <v>59793</v>
       </c>
       <c r="G55" t="n">
-        <v>-36225.56062979306</v>
+        <v>-5858.967081403262</v>
       </c>
       <c r="H55" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>-98408</v>
+        <v>-123590</v>
       </c>
       <c r="B56" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C56" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D56" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E56" t="n">
         <v>30000</v>
       </c>
       <c r="F56" t="n">
-        <v>49821</v>
+        <v>73697</v>
       </c>
       <c r="G56" t="n">
-        <v>-20649.95271615501</v>
+        <v>-32957.76361787422</v>
       </c>
       <c r="H56" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>-84710</v>
+        <v>-102216</v>
       </c>
       <c r="B57" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C57" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D57" t="n">
         <v>30000</v>
@@ -1923,62 +1923,62 @@
         <v>20000</v>
       </c>
       <c r="F57" t="n">
-        <v>69583</v>
+        <v>60634</v>
       </c>
       <c r="G57" t="n">
-        <v>-7854.951113873454</v>
+        <v>-44257.75054625681</v>
       </c>
       <c r="H57" t="n">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>-111088</v>
+        <v>-98368</v>
       </c>
       <c r="B58" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C58" t="n">
         <v>20000</v>
       </c>
       <c r="D58" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E58" t="n">
         <v>20000</v>
       </c>
       <c r="F58" t="n">
-        <v>49760</v>
+        <v>69843</v>
       </c>
       <c r="G58" t="n">
-        <v>-34293.48080365843</v>
+        <v>-35684.80991967075</v>
       </c>
       <c r="H58" t="n">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>-109386</v>
+        <v>-103011</v>
       </c>
       <c r="B59" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C59" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D59" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E59" t="n">
         <v>30000</v>
       </c>
       <c r="F59" t="n">
-        <v>38462</v>
+        <v>37999</v>
       </c>
       <c r="G59" t="n">
-        <v>-3689.701186961483</v>
+        <v>-22257.03500695468</v>
       </c>
       <c r="H59" t="n">
         <v>0.16</v>
@@ -1986,25 +1986,25 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>-122686</v>
+        <v>-82957</v>
       </c>
       <c r="B60" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="C60" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D60" t="n">
         <v>30000</v>
       </c>
       <c r="E60" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="F60" t="n">
-        <v>82570</v>
+        <v>58252</v>
       </c>
       <c r="G60" t="n">
-        <v>-53809.42562419607</v>
+        <v>3262.31616223245</v>
       </c>
       <c r="H60" t="n">
         <v>0.23</v>
@@ -2012,85 +2012,85 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>-109595</v>
+        <v>-107482</v>
       </c>
       <c r="B61" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C61" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D61" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E61" t="n">
         <v>60000</v>
       </c>
       <c r="F61" t="n">
-        <v>48825</v>
+        <v>48302</v>
       </c>
       <c r="G61" t="n">
-        <v>-6178.095393819345</v>
+        <v>-25683.01203099349</v>
       </c>
       <c r="H61" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>-104072</v>
+        <v>-104892</v>
       </c>
       <c r="B62" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C62" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D62" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="E62" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F62" t="n">
-        <v>80280</v>
+        <v>61554</v>
       </c>
       <c r="G62" t="n">
-        <v>-22988.77868804847</v>
+        <v>11862.83659074903</v>
       </c>
       <c r="H62" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>-107876</v>
+        <v>-107683</v>
       </c>
       <c r="B63" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C63" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D63" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E63" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F63" t="n">
-        <v>60258</v>
+        <v>60980</v>
       </c>
       <c r="G63" t="n">
-        <v>-14532.71956390169</v>
+        <v>-22197.72881890232</v>
       </c>
       <c r="H63" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>-102233</v>
+        <v>-100661</v>
       </c>
       <c r="B64" t="n">
         <v>40000</v>
@@ -2099,79 +2099,79 @@
         <v>20000</v>
       </c>
       <c r="D64" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E64" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F64" t="n">
-        <v>38521</v>
+        <v>79513</v>
       </c>
       <c r="G64" t="n">
-        <v>-39166.80598600775</v>
+        <v>-22452.53303651623</v>
       </c>
       <c r="H64" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>-99771</v>
+        <v>-122676</v>
       </c>
       <c r="B65" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C65" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D65" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E65" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F65" t="n">
-        <v>70397</v>
+        <v>57424</v>
       </c>
       <c r="G65" t="n">
-        <v>-22438.75428779523</v>
+        <v>-36097.5922565122</v>
       </c>
       <c r="H65" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>-111525</v>
+        <v>-90525</v>
       </c>
       <c r="B66" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C66" t="n">
         <v>30000</v>
       </c>
       <c r="D66" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="E66" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F66" t="n">
-        <v>61855</v>
+        <v>84313</v>
       </c>
       <c r="G66" t="n">
-        <v>-35439.73375493419</v>
+        <v>-7841.766647495111</v>
       </c>
       <c r="H66" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>-101415</v>
+        <v>-112361</v>
       </c>
       <c r="B67" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C67" t="n">
         <v>50000</v>
@@ -2183,50 +2183,50 @@
         <v>20000</v>
       </c>
       <c r="F67" t="n">
-        <v>61397</v>
+        <v>79205</v>
       </c>
       <c r="G67" t="n">
-        <v>-9367.177817888465</v>
+        <v>-7413.511190435212</v>
       </c>
       <c r="H67" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>-85190</v>
+        <v>-93480</v>
       </c>
       <c r="B68" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C68" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D68" t="n">
         <v>50000</v>
       </c>
       <c r="E68" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="F68" t="n">
-        <v>40002</v>
+        <v>78267</v>
       </c>
       <c r="G68" t="n">
-        <v>13348.60480388621</v>
+        <v>-18115.14517552148</v>
       </c>
       <c r="H68" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>-104133</v>
+        <v>-92821</v>
       </c>
       <c r="B69" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C69" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D69" t="n">
         <v>20000</v>
@@ -2235,270 +2235,270 @@
         <v>40000</v>
       </c>
       <c r="F69" t="n">
-        <v>84149</v>
+        <v>70414</v>
       </c>
       <c r="G69" t="n">
-        <v>-45208.8497139291</v>
+        <v>-15518.48479598922</v>
       </c>
       <c r="H69" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>-97956</v>
+        <v>-97223</v>
       </c>
       <c r="B70" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C70" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D70" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="E70" t="n">
         <v>50000</v>
       </c>
       <c r="F70" t="n">
-        <v>61799</v>
+        <v>78297</v>
       </c>
       <c r="G70" t="n">
-        <v>84.89259338754709</v>
+        <v>14377.98615090529</v>
       </c>
       <c r="H70" t="n">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>-102257</v>
+        <v>-110102</v>
       </c>
       <c r="B71" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C71" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D71" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="E71" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="F71" t="n">
-        <v>62765</v>
+        <v>39265</v>
       </c>
       <c r="G71" t="n">
-        <v>-22038.09805707802</v>
+        <v>-31190.80453137258</v>
       </c>
       <c r="H71" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>-94525</v>
+        <v>-116358</v>
       </c>
       <c r="B72" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C72" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D72" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E72" t="n">
         <v>30000</v>
       </c>
       <c r="F72" t="n">
-        <v>80007</v>
+        <v>77329</v>
       </c>
       <c r="G72" t="n">
-        <v>-3604.302928390087</v>
+        <v>-8636.64413565812</v>
       </c>
       <c r="H72" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>-107652</v>
+        <v>-92480</v>
       </c>
       <c r="B73" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C73" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D73" t="n">
         <v>50000</v>
       </c>
       <c r="E73" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F73" t="n">
-        <v>81299</v>
+        <v>40148</v>
       </c>
       <c r="G73" t="n">
-        <v>-29112.44957568174</v>
+        <v>-22931.14175178952</v>
       </c>
       <c r="H73" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>-86743</v>
+        <v>-92658</v>
       </c>
       <c r="B74" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C74" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D74" t="n">
         <v>50000</v>
       </c>
       <c r="E74" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F74" t="n">
-        <v>72662</v>
+        <v>69195</v>
       </c>
       <c r="G74" t="n">
-        <v>20637.8699335292</v>
+        <v>-9027.310558251371</v>
       </c>
       <c r="H74" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>-99787</v>
+        <v>-118666</v>
       </c>
       <c r="B75" t="n">
         <v>40000</v>
       </c>
       <c r="C75" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D75" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E75" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F75" t="n">
-        <v>44801</v>
+        <v>80976</v>
       </c>
       <c r="G75" t="n">
-        <v>-5950.952261871336</v>
+        <v>-34823.14012616677</v>
       </c>
       <c r="H75" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>-103872</v>
+        <v>-109614</v>
       </c>
       <c r="B76" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C76" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D76" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="E76" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F76" t="n">
-        <v>70082</v>
+        <v>49262</v>
       </c>
       <c r="G76" t="n">
-        <v>-12475.1461282523</v>
+        <v>-17428.805646381</v>
       </c>
       <c r="H76" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>-111502</v>
+        <v>-86593</v>
       </c>
       <c r="B77" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C77" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="D77" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E77" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F77" t="n">
-        <v>45605</v>
+        <v>61410</v>
       </c>
       <c r="G77" t="n">
-        <v>-7524.752614985196</v>
+        <v>-24841.04355177775</v>
       </c>
       <c r="H77" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>-85191</v>
+        <v>-119540</v>
       </c>
       <c r="B78" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="C78" t="n">
         <v>40000</v>
       </c>
       <c r="D78" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E78" t="n">
         <v>60000</v>
       </c>
       <c r="F78" t="n">
-        <v>72883</v>
+        <v>71083</v>
       </c>
       <c r="G78" t="n">
-        <v>10637.778293424</v>
+        <v>-38440.2707131799</v>
       </c>
       <c r="H78" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>-95328</v>
+        <v>-95725</v>
       </c>
       <c r="B79" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C79" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D79" t="n">
         <v>60000</v>
       </c>
       <c r="E79" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F79" t="n">
-        <v>70415</v>
+        <v>78367</v>
       </c>
       <c r="G79" t="n">
-        <v>-4347.909407562793</v>
+        <v>23592.97811870594</v>
       </c>
       <c r="H79" t="n">
         <v>0.18</v>
@@ -2506,51 +2506,51 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>-99296</v>
+        <v>-101448</v>
       </c>
       <c r="B80" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C80" t="n">
         <v>40000</v>
       </c>
       <c r="D80" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="E80" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="F80" t="n">
-        <v>54544</v>
+        <v>52332</v>
       </c>
       <c r="G80" t="n">
-        <v>-30961.75915908266</v>
+        <v>-23343.77861212401</v>
       </c>
       <c r="H80" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>-93053</v>
+        <v>-122453</v>
       </c>
       <c r="B81" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C81" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D81" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E81" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F81" t="n">
-        <v>70103</v>
+        <v>39357</v>
       </c>
       <c r="G81" t="n">
-        <v>-9148.782541272203</v>
+        <v>-19806.71486479262</v>
       </c>
       <c r="H81" t="n">
         <v>0.21</v>
@@ -2558,267 +2558,267 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>-117936</v>
+        <v>-118948</v>
       </c>
       <c r="B82" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C82" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="D82" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E82" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F82" t="n">
-        <v>82948</v>
+        <v>58479</v>
       </c>
       <c r="G82" t="n">
-        <v>-44809.74190874083</v>
+        <v>-7440.737809907556</v>
       </c>
       <c r="H82" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>-99031</v>
+        <v>-112911</v>
       </c>
       <c r="B83" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C83" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D83" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E83" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F83" t="n">
-        <v>49880</v>
+        <v>74197</v>
       </c>
       <c r="G83" t="n">
-        <v>-12826.4106962239</v>
+        <v>-22535.83287937765</v>
       </c>
       <c r="H83" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>-104118</v>
+        <v>-107182</v>
       </c>
       <c r="B84" t="n">
         <v>60000</v>
       </c>
       <c r="C84" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D84" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E84" t="n">
         <v>30000</v>
       </c>
       <c r="F84" t="n">
-        <v>79696</v>
+        <v>69934</v>
       </c>
       <c r="G84" t="n">
-        <v>-14804.16529652924</v>
+        <v>-8126.32052205621</v>
       </c>
       <c r="H84" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>-119901</v>
+        <v>-111951</v>
       </c>
       <c r="B85" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C85" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D85" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E85" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F85" t="n">
-        <v>77882</v>
+        <v>81060</v>
       </c>
       <c r="G85" t="n">
-        <v>-17022.39878298615</v>
+        <v>-17256.92459371477</v>
       </c>
       <c r="H85" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>-96642</v>
+        <v>-94924</v>
       </c>
       <c r="B86" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="C86" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="D86" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E86" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="F86" t="n">
-        <v>40780</v>
+        <v>73564</v>
       </c>
       <c r="G86" t="n">
-        <v>17856.1768520805</v>
+        <v>-4164.583953664483</v>
       </c>
       <c r="H86" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>-108671</v>
+        <v>-114691</v>
       </c>
       <c r="B87" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="C87" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D87" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="E87" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F87" t="n">
-        <v>85111</v>
+        <v>39003</v>
       </c>
       <c r="G87" t="n">
-        <v>-5477.851372936781</v>
+        <v>-44304.40050031693</v>
       </c>
       <c r="H87" t="n">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>-92015</v>
+        <v>-106906</v>
       </c>
       <c r="B88" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C88" t="n">
         <v>20000</v>
       </c>
       <c r="D88" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E88" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F88" t="n">
-        <v>39866</v>
+        <v>42099</v>
       </c>
       <c r="G88" t="n">
-        <v>-12408.97367797419</v>
+        <v>-39809.58704528697</v>
       </c>
       <c r="H88" t="n">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>-93310</v>
+        <v>-117093</v>
       </c>
       <c r="B89" t="n">
         <v>30000</v>
       </c>
       <c r="C89" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="D89" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E89" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F89" t="n">
-        <v>78654</v>
+        <v>61948</v>
       </c>
       <c r="G89" t="n">
-        <v>-5562.259564705952</v>
+        <v>-39914.20823139868</v>
       </c>
       <c r="H89" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>-101322</v>
+        <v>-91583</v>
       </c>
       <c r="B90" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C90" t="n">
         <v>50000</v>
       </c>
       <c r="D90" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E90" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F90" t="n">
-        <v>82433</v>
+        <v>44051</v>
       </c>
       <c r="G90" t="n">
-        <v>-29329.21262675518</v>
+        <v>3907.841549365674</v>
       </c>
       <c r="H90" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>-122992</v>
+        <v>-107429</v>
       </c>
       <c r="B91" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="C91" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D91" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="E91" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F91" t="n">
-        <v>40297</v>
+        <v>70148</v>
       </c>
       <c r="G91" t="n">
-        <v>-47868.62560060346</v>
+        <v>-2696.882185502751</v>
       </c>
       <c r="H91" t="n">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>-123334</v>
+        <v>-99274</v>
       </c>
       <c r="B92" t="n">
         <v>20000</v>
@@ -2827,94 +2827,94 @@
         <v>50000</v>
       </c>
       <c r="D92" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="E92" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F92" t="n">
-        <v>79453</v>
+        <v>61215</v>
       </c>
       <c r="G92" t="n">
-        <v>-36315.94691578385</v>
+        <v>-17347.42030899207</v>
       </c>
       <c r="H92" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>-101638</v>
+        <v>-113308</v>
       </c>
       <c r="B93" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C93" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="D93" t="n">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E93" t="n">
         <v>50000</v>
       </c>
       <c r="F93" t="n">
-        <v>57987</v>
+        <v>62986</v>
       </c>
       <c r="G93" t="n">
-        <v>-14636.90119827544</v>
+        <v>-27691.9018197805</v>
       </c>
       <c r="H93" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>-106539</v>
+        <v>-114673</v>
       </c>
       <c r="B94" t="n">
         <v>50000</v>
       </c>
       <c r="C94" t="n">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="D94" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E94" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F94" t="n">
-        <v>42724</v>
+        <v>49452</v>
       </c>
       <c r="G94" t="n">
-        <v>-13118.30207536499</v>
+        <v>-14229.61941243615</v>
       </c>
       <c r="H94" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>-120448</v>
+        <v>-105322</v>
       </c>
       <c r="B95" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="C95" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="D95" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="E95" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F95" t="n">
-        <v>39760</v>
+        <v>79752</v>
       </c>
       <c r="G95" t="n">
-        <v>-55079.4924621531</v>
+        <v>-6038.856169558705</v>
       </c>
       <c r="H95" t="n">
         <v>0.18</v>
@@ -2922,25 +2922,25 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>-102642</v>
+        <v>-121332</v>
       </c>
       <c r="B96" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="C96" t="n">
         <v>60000</v>
       </c>
       <c r="D96" t="n">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="E96" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="F96" t="n">
-        <v>41874</v>
+        <v>69763</v>
       </c>
       <c r="G96" t="n">
-        <v>-2019.837214949564</v>
+        <v>-4063.793952040522</v>
       </c>
       <c r="H96" t="n">
         <v>0.2</v>
@@ -2948,77 +2948,77 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>-108153</v>
+        <v>-93192</v>
       </c>
       <c r="B97" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C97" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D97" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E97" t="n">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="F97" t="n">
-        <v>71732</v>
+        <v>83270</v>
       </c>
       <c r="G97" t="n">
-        <v>-11495.85569376033</v>
+        <v>-30426.52470261193</v>
       </c>
       <c r="H97" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>-98662</v>
+        <v>-126716</v>
       </c>
       <c r="B98" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C98" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D98" t="n">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E98" t="n">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="F98" t="n">
-        <v>43165</v>
+        <v>42249</v>
       </c>
       <c r="G98" t="n">
-        <v>-43065.62157124485</v>
+        <v>-45213.20973847307</v>
       </c>
       <c r="H98" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>-104271</v>
+        <v>-86789</v>
       </c>
       <c r="B99" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C99" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D99" t="n">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E99" t="n">
         <v>30000</v>
       </c>
       <c r="F99" t="n">
-        <v>41432</v>
+        <v>79267</v>
       </c>
       <c r="G99" t="n">
-        <v>-4303.062048524102</v>
+        <v>-2721.960359103765</v>
       </c>
       <c r="H99" t="n">
         <v>0.21</v>
@@ -3026,54 +3026,54 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>-107087</v>
+        <v>-100893</v>
       </c>
       <c r="B100" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="C100" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D100" t="n">
         <v>20000</v>
       </c>
       <c r="E100" t="n">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="F100" t="n">
-        <v>40910</v>
+        <v>80505</v>
       </c>
       <c r="G100" t="n">
-        <v>-41777.53063166965</v>
+        <v>-13011.28953174854</v>
       </c>
       <c r="H100" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>-96622</v>
+        <v>-90510</v>
       </c>
       <c r="B101" t="n">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="C101" t="n">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="D101" t="n">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="E101" t="n">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F101" t="n">
-        <v>59902</v>
+        <v>56788</v>
       </c>
       <c r="G101" t="n">
-        <v>-17868.5804609649</v>
+        <v>-22760.10679069255</v>
       </c>
       <c r="H101" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>